<commit_message>
TS 1.2 Tamil Ghanam files 07/09/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A26F05-45E0-4044-9100-5CFD49AD7700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -3067,7 +3068,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="171" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4559,6 +4560,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4594,6 +4612,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4769,7 +4804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9557,7 +9592,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1"/>
+    <hyperlink ref="I7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -9565,7 +9600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12467,7 +12502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
@@ -14584,7 +14619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17571,7 +17606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21743,7 +21778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23878,7 +23913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Shanti Japam sans corr - 27/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D9D014-08CD-4BF8-910A-F4E6067AEC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092F16CD-AF7F-4B8E-8160-D7222FE89150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1015">
   <si>
     <t>Date</t>
   </si>
@@ -3082,13 +3082,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="172" x14ac:knownFonts="1">
+  <fonts count="174" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4162,72 +4174,74 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="171" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="167" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="168" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="169" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="170" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="168" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="170" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="167" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="169" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="168" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="170" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="160" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="157" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="160" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="151" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="150" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="137" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="169" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="171" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="169" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="169" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="171" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="171" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="134" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4235,18 +4249,18 @@
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="124" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="120" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4260,19 +4274,19 @@
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="104" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="168" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="170" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4288,30 +4302,30 @@
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4324,168 +4338,169 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="109" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="107" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="106" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="107" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="105" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="104" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="168" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="172" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="172" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="170" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="103" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="167" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="169" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="167" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="169" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="81" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14642,7 +14657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -17631,8 +17646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17721,7 +17736,7 @@
       <c r="H4" s="200" t="s">
         <v>152</v>
       </c>
-      <c r="I4" s="68" t="s">
+      <c r="I4" s="242" t="s">
         <v>569</v>
       </c>
     </row>
@@ -17766,7 +17781,9 @@
       <c r="H6" s="88" t="s">
         <v>571</v>
       </c>
-      <c r="I6" s="68"/>
+      <c r="I6" s="241" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="88"/>
@@ -17802,7 +17819,7 @@
         <v>15.3</v>
       </c>
       <c r="H8" s="88"/>
-      <c r="I8" s="88" t="s">
+      <c r="I8" s="242" t="s">
         <v>573</v>
       </c>
     </row>
@@ -17868,7 +17885,9 @@
       <c r="H11" s="94" t="s">
         <v>578</v>
       </c>
-      <c r="I11" s="88"/>
+      <c r="I11" s="241" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="88"/>
@@ -17904,7 +17923,7 @@
         <v>15.02</v>
       </c>
       <c r="H13" s="88"/>
-      <c r="I13" s="88" t="s">
+      <c r="I13" s="242" t="s">
         <v>580</v>
       </c>
     </row>
@@ -17950,7 +17969,9 @@
       <c r="H15" s="94" t="s">
         <v>582</v>
       </c>
-      <c r="I15" s="88"/>
+      <c r="I15" s="243" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="88"/>
@@ -17986,7 +18007,7 @@
         <v>9.43</v>
       </c>
       <c r="H17" s="88"/>
-      <c r="I17" s="88" t="s">
+      <c r="I17" s="242" t="s">
         <v>584</v>
       </c>
     </row>
@@ -21794,8 +21815,14 @@
       <c r="I236" s="88"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{F98ED066-CB19-4B46-8CC6-0978F01090BC}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{7A24F6C1-A105-4B74-A527-D47A71FE5DCB}"/>
+    <hyperlink ref="I13" r:id="rId3" xr:uid="{24E77FE3-7C84-4E8F-849A-A8579B12B0B4}"/>
+    <hyperlink ref="I17" r:id="rId4" xr:uid="{6DCA4BCF-B88C-468C-88BF-CF86647D06D4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 5.5 to 5.7 updates - 09-05-2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50AB8DC-1A9E-4900-AFE4-E814310FBCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D902C-4A27-423B-919C-443BBB59E907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="1015">
   <si>
     <t>Date</t>
   </si>
@@ -3082,13 +3082,37 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="185" x14ac:knownFonts="1">
+  <fonts count="189" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4240,49 +4264,54 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="180" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="181" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="181" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="180" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="181" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="185" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="177" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="174" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="173" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="177" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="173" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="166" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="165" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="157" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="157" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4290,41 +4319,40 @@
     <xf numFmtId="2" fontId="152" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="186" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="186" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="182" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="182" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="182" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="140" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="136" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="131" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="131" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4336,21 +4364,21 @@
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="185" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="115" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="181" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4364,32 +4392,32 @@
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="87" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4400,170 +4428,170 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="63" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="57" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="124" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="122" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="121" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="120" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="118" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="117" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="183" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="183" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="181" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="180" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="180" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17722,8 +17750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19431,7 +19459,9 @@
       <c r="H81" s="110" t="s">
         <v>652</v>
       </c>
-      <c r="I81" s="88"/>
+      <c r="I81" s="254" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="88"/>
@@ -19552,7 +19582,9 @@
       <c r="G87" s="88">
         <v>56.54</v>
       </c>
-      <c r="H87" s="88"/>
+      <c r="H87" s="255" t="s">
+        <v>865</v>
+      </c>
       <c r="I87" s="88"/>
     </row>
     <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -19779,7 +19811,9 @@
       <c r="G98" s="88">
         <v>56.17</v>
       </c>
-      <c r="H98" s="88"/>
+      <c r="H98" s="256" t="s">
+        <v>865</v>
+      </c>
       <c r="I98" s="88"/>
     </row>
     <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -19922,7 +19956,9 @@
       <c r="G105" s="93">
         <v>12.51</v>
       </c>
-      <c r="H105" s="88"/>
+      <c r="H105" s="257" t="s">
+        <v>865</v>
+      </c>
       <c r="I105" s="88"/>
     </row>
     <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20009,7 +20045,9 @@
       <c r="H109" s="114" t="s">
         <v>683</v>
       </c>
-      <c r="I109" s="88"/>
+      <c r="I109" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="88"/>

</xml_diff>

<commit_message>
TS 5.6 5.7 Templates listening corr - 10/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D902C-4A27-423B-919C-443BBB59E907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DFDD42-335A-4D30-B2A9-C6C2AE1F587C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="1015">
   <si>
     <t>Date</t>
   </si>
@@ -3082,13 +3082,37 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="189" x14ac:knownFonts="1">
+  <fonts count="193" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4264,49 +4288,54 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="189" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="189" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="185" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="189" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="181" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="178" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="177" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="181" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="174" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="177" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="169" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="166" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="165" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="165" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="160" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4314,41 +4343,40 @@
     <xf numFmtId="2" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="190" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="190" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="153" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="153" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="152" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="186" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="186" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="186" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="143" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="140" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="139" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="135" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4360,21 +4388,21 @@
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="123" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="189" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="119" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="185" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4388,32 +4416,32 @@
     <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="95" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="93" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="91" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4424,170 +4452,170 @@
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="69" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="65" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="128" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="126" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="125" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="124" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="122" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="121" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="185" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="118" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="189" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="122" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17751,7 +17779,7 @@
   <dimension ref="A1:I236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+      <selection activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20171,7 +20199,9 @@
       <c r="H115" s="114" t="s">
         <v>688</v>
       </c>
-      <c r="I115" s="88"/>
+      <c r="I115" s="258" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="88"/>
@@ -20250,7 +20280,9 @@
       <c r="G119" s="88">
         <v>35.32</v>
       </c>
-      <c r="H119" s="88"/>
+      <c r="H119" s="259" t="s">
+        <v>865</v>
+      </c>
       <c r="I119" s="88"/>
     </row>
     <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20460,7 +20492,9 @@
       <c r="G129" s="88">
         <v>55.55</v>
       </c>
-      <c r="H129" s="88"/>
+      <c r="H129" s="260" t="s">
+        <v>865</v>
+      </c>
       <c r="I129" s="88"/>
     </row>
     <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20627,7 +20661,9 @@
       <c r="H137" s="117" t="s">
         <v>716</v>
       </c>
-      <c r="I137" s="88"/>
+      <c r="I137" s="261" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="88"/>

</xml_diff>

<commit_message>
TS Pada Paatam analysis - 13/05/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31EB07F-8316-4C06-B3D2-C08E001ADF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5D698-B868-4FB2-ABAA-A982772AABB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -3082,7 +3082,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="195" x14ac:knownFonts="1">
+  <fonts count="194" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4248,14 +4248,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -4298,11 +4290,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="190" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4545,9 +4536,6 @@
     <xf numFmtId="2" fontId="190" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4648,8 +4636,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4988,10 +4975,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5001,7 +4988,7 @@
     <col min="3" max="3" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="7" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="239" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="238" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="7" customWidth="1"/>
     <col min="9" max="9" width="64.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="7"/>
@@ -5084,7 +5071,7 @@
         <v>8.44</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="214" t="s">
+      <c r="I7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="4"/>
@@ -5173,7 +5160,7 @@
       <c r="G11" s="213">
         <v>33.380000000000003</v>
       </c>
-      <c r="H11" s="215"/>
+      <c r="H11" s="214"/>
       <c r="I11" s="4" t="s">
         <v>67</v>
       </c>
@@ -5286,7 +5273,7 @@
       <c r="G16" s="213">
         <v>30.56</v>
       </c>
-      <c r="H16" s="216"/>
+      <c r="H16" s="215"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -5329,7 +5316,7 @@
       <c r="G18" s="213">
         <v>52.12</v>
       </c>
-      <c r="H18" s="217"/>
+      <c r="H18" s="216"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -5419,7 +5406,7 @@
       <c r="G22" s="213">
         <v>29.49</v>
       </c>
-      <c r="H22" s="218"/>
+      <c r="H22" s="217"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -5488,7 +5475,7 @@
       <c r="G25" s="213">
         <v>49.18</v>
       </c>
-      <c r="H25" s="219" t="s">
+      <c r="H25" s="218" t="s">
         <v>28</v>
       </c>
       <c r="I25" s="4"/>
@@ -5807,7 +5794,7 @@
         <f>+D38+1</f>
         <v>4</v>
       </c>
-      <c r="E39" s="220" t="s">
+      <c r="E39" s="219" t="s">
         <v>759</v>
       </c>
       <c r="F39" s="213">
@@ -5817,7 +5804,7 @@
       <c r="G39" s="213">
         <v>51.4</v>
       </c>
-      <c r="H39" s="221" t="s">
+      <c r="H39" s="220" t="s">
         <v>46</v>
       </c>
       <c r="I39" s="4"/>
@@ -6221,7 +6208,7 @@
       <c r="G56" s="213">
         <v>50.43</v>
       </c>
-      <c r="H56" s="219" t="s">
+      <c r="H56" s="218" t="s">
         <v>209</v>
       </c>
       <c r="I56" s="4"/>
@@ -6532,7 +6519,7 @@
       <c r="G69" s="213">
         <v>53.12</v>
       </c>
-      <c r="H69" s="222" t="s">
+      <c r="H69" s="221" t="s">
         <v>668</v>
       </c>
       <c r="I69" s="4"/>
@@ -7286,7 +7273,7 @@
       <c r="G106" s="213">
         <v>47.51</v>
       </c>
-      <c r="H106" s="223" t="s">
+      <c r="H106" s="222" t="s">
         <v>779</v>
       </c>
       <c r="I106" s="4"/>
@@ -7385,7 +7372,7 @@
       <c r="G111" s="213">
         <v>53.04</v>
       </c>
-      <c r="H111" s="224"/>
+      <c r="H111" s="223"/>
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -7482,7 +7469,7 @@
       <c r="G116" s="213">
         <v>55.39</v>
       </c>
-      <c r="H116" s="225" t="s">
+      <c r="H116" s="224" t="s">
         <v>849</v>
       </c>
       <c r="I116" s="4"/>
@@ -7504,7 +7491,7 @@
       <c r="B118" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C118" s="226" t="s">
+      <c r="C118" s="225" t="s">
         <v>655</v>
       </c>
       <c r="D118" s="4">
@@ -7562,7 +7549,7 @@
       <c r="G120" s="213">
         <v>47.24</v>
       </c>
-      <c r="H120" s="227"/>
+      <c r="H120" s="226"/>
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -7582,7 +7569,7 @@
       <c r="G121" s="213">
         <v>59.38</v>
       </c>
-      <c r="H121" s="219" t="s">
+      <c r="H121" s="218" t="s">
         <v>208</v>
       </c>
       <c r="I121" s="4"/>
@@ -7619,7 +7606,7 @@
       <c r="G123" s="213">
         <v>5.59</v>
       </c>
-      <c r="H123" s="224" t="s">
+      <c r="H123" s="223" t="s">
         <v>848</v>
       </c>
       <c r="I123" s="4" t="s">
@@ -7643,7 +7630,7 @@
       <c r="G124" s="213">
         <v>15.35</v>
       </c>
-      <c r="H124" s="228" t="s">
+      <c r="H124" s="227" t="s">
         <v>152</v>
       </c>
       <c r="I124" s="4"/>
@@ -7704,7 +7691,7 @@
       <c r="G127" s="213">
         <v>56.45</v>
       </c>
-      <c r="H127" s="229" t="s">
+      <c r="H127" s="228" t="s">
         <v>865</v>
       </c>
       <c r="I127" s="4"/>
@@ -7723,16 +7710,16 @@
       <c r="A129" s="4">
         <v>12</v>
       </c>
-      <c r="B129" s="230" t="s">
+      <c r="B129" s="229" t="s">
         <v>147</v>
       </c>
-      <c r="C129" s="230" t="s">
+      <c r="C129" s="229" t="s">
         <v>149</v>
       </c>
       <c r="D129" s="4">
         <v>1</v>
       </c>
-      <c r="E129" s="230" t="s">
+      <c r="E129" s="229" t="s">
         <v>148</v>
       </c>
       <c r="F129" s="213">
@@ -7753,7 +7740,7 @@
         <f>+D129+1</f>
         <v>2</v>
       </c>
-      <c r="E130" s="230" t="s">
+      <c r="E130" s="229" t="s">
         <v>151</v>
       </c>
       <c r="F130" s="213">
@@ -7763,7 +7750,7 @@
       <c r="G130" s="213">
         <v>25</v>
       </c>
-      <c r="H130" s="230" t="s">
+      <c r="H130" s="229" t="s">
         <v>152</v>
       </c>
       <c r="I130" s="4"/>
@@ -7775,7 +7762,7 @@
         <f>+D130+1</f>
         <v>3</v>
       </c>
-      <c r="E131" s="230" t="s">
+      <c r="E131" s="229" t="s">
         <v>153</v>
       </c>
       <c r="F131" s="213">
@@ -7794,7 +7781,7 @@
         <f>+D131+1</f>
         <v>4</v>
       </c>
-      <c r="E132" s="230" t="s">
+      <c r="E132" s="229" t="s">
         <v>154</v>
       </c>
       <c r="F132" s="213">
@@ -7814,7 +7801,7 @@
         <f>+D132+1</f>
         <v>5</v>
       </c>
-      <c r="E133" s="230" t="s">
+      <c r="E133" s="229" t="s">
         <v>155</v>
       </c>
       <c r="F133" s="213">
@@ -7824,7 +7811,7 @@
       <c r="G133" s="213">
         <v>59.01</v>
       </c>
-      <c r="H133" s="231" t="s">
+      <c r="H133" s="230" t="s">
         <v>866</v>
       </c>
       <c r="I133" s="4"/>
@@ -7843,7 +7830,7 @@
       <c r="A135" s="4">
         <v>13</v>
       </c>
-      <c r="B135" s="230" t="s">
+      <c r="B135" s="229" t="s">
         <v>156</v>
       </c>
       <c r="C135" s="4">
@@ -7852,7 +7839,7 @@
       <c r="D135" s="4">
         <v>1</v>
       </c>
-      <c r="E135" s="230" t="s">
+      <c r="E135" s="229" t="s">
         <v>158</v>
       </c>
       <c r="F135" s="213">
@@ -7873,7 +7860,7 @@
         <f t="shared" ref="D136:D141" si="11">+D135+1</f>
         <v>2</v>
       </c>
-      <c r="E136" s="230" t="s">
+      <c r="E136" s="229" t="s">
         <v>159</v>
       </c>
       <c r="F136" s="213">
@@ -7893,7 +7880,7 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="E137" s="219" t="s">
+      <c r="E137" s="218" t="s">
         <v>207</v>
       </c>
       <c r="F137" s="213">
@@ -7902,7 +7889,7 @@
       <c r="G137" s="213">
         <v>54.17</v>
       </c>
-      <c r="H137" s="219" t="s">
+      <c r="H137" s="218" t="s">
         <v>160</v>
       </c>
       <c r="I137" s="4"/>
@@ -7921,7 +7908,7 @@
       <c r="A139" s="4">
         <v>14</v>
       </c>
-      <c r="B139" s="230" t="s">
+      <c r="B139" s="229" t="s">
         <v>161</v>
       </c>
       <c r="C139" s="4">
@@ -7930,7 +7917,7 @@
       <c r="D139" s="4">
         <v>1</v>
       </c>
-      <c r="E139" s="230" t="s">
+      <c r="E139" s="229" t="s">
         <v>163</v>
       </c>
       <c r="F139" s="213">
@@ -7951,7 +7938,7 @@
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="E140" s="230" t="s">
+      <c r="E140" s="229" t="s">
         <v>165</v>
       </c>
       <c r="F140" s="213">
@@ -7961,7 +7948,7 @@
       <c r="G140" s="213">
         <v>26.55</v>
       </c>
-      <c r="H140" s="232" t="s">
+      <c r="H140" s="231" t="s">
         <v>943</v>
       </c>
       <c r="I140" s="4"/>
@@ -7973,7 +7960,7 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="E141" s="230" t="s">
+      <c r="E141" s="229" t="s">
         <v>168</v>
       </c>
       <c r="F141" s="213">
@@ -7991,7 +7978,7 @@
       <c r="D142" s="4">
         <v>4</v>
       </c>
-      <c r="E142" s="230" t="s">
+      <c r="E142" s="229" t="s">
         <v>169</v>
       </c>
       <c r="F142" s="213">
@@ -8001,7 +7988,7 @@
       <c r="G142" s="213">
         <v>51.34</v>
       </c>
-      <c r="H142" s="219" t="s">
+      <c r="H142" s="218" t="s">
         <v>169</v>
       </c>
       <c r="I142" s="4"/>
@@ -8020,7 +8007,7 @@
       <c r="A144" s="4">
         <v>15</v>
       </c>
-      <c r="B144" s="230" t="s">
+      <c r="B144" s="229" t="s">
         <v>166</v>
       </c>
       <c r="C144" s="4">
@@ -8029,7 +8016,7 @@
       <c r="D144" s="4">
         <v>1</v>
       </c>
-      <c r="E144" s="230" t="s">
+      <c r="E144" s="229" t="s">
         <v>170</v>
       </c>
       <c r="F144" s="213">
@@ -8050,7 +8037,7 @@
         <f>+D144+1</f>
         <v>2</v>
       </c>
-      <c r="E145" s="230" t="s">
+      <c r="E145" s="229" t="s">
         <v>171</v>
       </c>
       <c r="F145" s="213">
@@ -8064,14 +8051,14 @@
       <c r="I145" s="4"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B146" s="233" t="s">
+      <c r="B146" s="232" t="s">
         <v>865</v>
       </c>
       <c r="C146" s="4"/>
       <c r="D146" s="4">
         <v>3</v>
       </c>
-      <c r="E146" s="230" t="s">
+      <c r="E146" s="229" t="s">
         <v>172</v>
       </c>
       <c r="F146" s="213">
@@ -8098,7 +8085,7 @@
       <c r="A148" s="4">
         <v>16</v>
       </c>
-      <c r="B148" s="230" t="s">
+      <c r="B148" s="229" t="s">
         <v>173</v>
       </c>
       <c r="C148" s="4">
@@ -8107,7 +8094,7 @@
       <c r="D148" s="4">
         <v>1</v>
       </c>
-      <c r="E148" s="230" t="s">
+      <c r="E148" s="229" t="s">
         <v>174</v>
       </c>
       <c r="F148" s="213">
@@ -8128,7 +8115,7 @@
         <f>+D148+1</f>
         <v>2</v>
       </c>
-      <c r="E149" s="234" t="s">
+      <c r="E149" s="233" t="s">
         <v>175</v>
       </c>
       <c r="F149" s="213">
@@ -8148,7 +8135,7 @@
         <f>+D149+1</f>
         <v>3</v>
       </c>
-      <c r="E150" s="234" t="s">
+      <c r="E150" s="233" t="s">
         <v>176</v>
       </c>
       <c r="F150" s="213">
@@ -8168,7 +8155,7 @@
         <f>+D150+1</f>
         <v>4</v>
       </c>
-      <c r="E151" s="234" t="s">
+      <c r="E151" s="233" t="s">
         <v>177</v>
       </c>
       <c r="F151" s="213">
@@ -8182,7 +8169,7 @@
       <c r="I151" s="4"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B152" s="235" t="s">
+      <c r="B152" s="234" t="s">
         <v>865</v>
       </c>
       <c r="C152" s="4"/>
@@ -8190,7 +8177,7 @@
         <f>+D151+1</f>
         <v>5</v>
       </c>
-      <c r="E152" s="234" t="s">
+      <c r="E152" s="233" t="s">
         <v>178</v>
       </c>
       <c r="F152" s="213">
@@ -8200,7 +8187,7 @@
       <c r="G152" s="213">
         <v>55.39</v>
       </c>
-      <c r="H152" s="219" t="s">
+      <c r="H152" s="218" t="s">
         <v>178</v>
       </c>
       <c r="I152" s="4"/>
@@ -8219,7 +8206,7 @@
       <c r="A154" s="4">
         <v>17</v>
       </c>
-      <c r="B154" s="234" t="s">
+      <c r="B154" s="233" t="s">
         <v>180</v>
       </c>
       <c r="C154" s="4">
@@ -8228,7 +8215,7 @@
       <c r="D154" s="4">
         <v>1</v>
       </c>
-      <c r="E154" s="234" t="s">
+      <c r="E154" s="233" t="s">
         <v>181</v>
       </c>
       <c r="F154" s="213">
@@ -8249,7 +8236,7 @@
         <f>+D154+1</f>
         <v>2</v>
       </c>
-      <c r="E155" s="234" t="s">
+      <c r="E155" s="233" t="s">
         <v>182</v>
       </c>
       <c r="F155" s="213">
@@ -8269,7 +8256,7 @@
         <f>+D155+1</f>
         <v>3</v>
       </c>
-      <c r="E156" s="234" t="s">
+      <c r="E156" s="233" t="s">
         <v>183</v>
       </c>
       <c r="F156" s="213">
@@ -8289,7 +8276,7 @@
         <f>+D156+1</f>
         <v>4</v>
       </c>
-      <c r="E157" s="234" t="s">
+      <c r="E157" s="233" t="s">
         <v>184</v>
       </c>
       <c r="F157" s="213">
@@ -8309,7 +8296,7 @@
         <f>+D157+1</f>
         <v>5</v>
       </c>
-      <c r="E158" s="234" t="s">
+      <c r="E158" s="233" t="s">
         <v>185</v>
       </c>
       <c r="F158" s="213">
@@ -8328,7 +8315,7 @@
         <f>+D158+1</f>
         <v>6</v>
       </c>
-      <c r="E159" s="234" t="s">
+      <c r="E159" s="233" t="s">
         <v>186</v>
       </c>
       <c r="F159" s="213">
@@ -8338,7 +8325,7 @@
       <c r="G159" s="213">
         <v>53.04</v>
       </c>
-      <c r="H159" s="219" t="s">
+      <c r="H159" s="218" t="s">
         <v>206</v>
       </c>
       <c r="I159" s="4"/>
@@ -8357,7 +8344,7 @@
       <c r="A161" s="4">
         <v>18</v>
       </c>
-      <c r="B161" s="234" t="s">
+      <c r="B161" s="233" t="s">
         <v>188</v>
       </c>
       <c r="C161" s="4">
@@ -8366,7 +8353,7 @@
       <c r="D161" s="4">
         <v>1</v>
       </c>
-      <c r="E161" s="234" t="s">
+      <c r="E161" s="233" t="s">
         <v>189</v>
       </c>
       <c r="F161" s="213">
@@ -8375,7 +8362,7 @@
       <c r="G161" s="213">
         <v>15.05</v>
       </c>
-      <c r="H161" s="236" t="s">
+      <c r="H161" s="235" t="s">
         <v>865</v>
       </c>
       <c r="I161" s="4" t="s">
@@ -8389,7 +8376,7 @@
         <f t="shared" ref="D162:D167" si="12">+D161+1</f>
         <v>2</v>
       </c>
-      <c r="E162" s="234" t="s">
+      <c r="E162" s="233" t="s">
         <v>191</v>
       </c>
       <c r="F162" s="213">
@@ -8409,7 +8396,7 @@
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="E163" s="234" t="s">
+      <c r="E163" s="233" t="s">
         <v>192</v>
       </c>
       <c r="F163" s="213">
@@ -8429,7 +8416,7 @@
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="E164" s="234" t="s">
+      <c r="E164" s="233" t="s">
         <v>193</v>
       </c>
       <c r="F164" s="213">
@@ -8449,7 +8436,7 @@
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="E165" s="234" t="s">
+      <c r="E165" s="233" t="s">
         <v>194</v>
       </c>
       <c r="F165" s="213">
@@ -8469,7 +8456,7 @@
         <f t="shared" si="12"/>
         <v>6</v>
       </c>
-      <c r="E166" s="234" t="s">
+      <c r="E166" s="233" t="s">
         <v>195</v>
       </c>
       <c r="F166" s="213">
@@ -8489,7 +8476,7 @@
         <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="E167" s="234" t="s">
+      <c r="E167" s="233" t="s">
         <v>196</v>
       </c>
       <c r="F167" s="213">
@@ -8516,7 +8503,7 @@
       <c r="A169" s="4">
         <v>19</v>
       </c>
-      <c r="B169" s="234" t="s">
+      <c r="B169" s="233" t="s">
         <v>197</v>
       </c>
       <c r="C169" s="213">
@@ -8525,7 +8512,7 @@
       <c r="D169" s="4">
         <v>1</v>
       </c>
-      <c r="E169" s="234" t="s">
+      <c r="E169" s="233" t="s">
         <v>199</v>
       </c>
       <c r="F169" s="213">
@@ -8546,7 +8533,7 @@
         <f>+D169+1</f>
         <v>2</v>
       </c>
-      <c r="E170" s="234" t="s">
+      <c r="E170" s="233" t="s">
         <v>200</v>
       </c>
       <c r="F170" s="213">
@@ -8566,7 +8553,7 @@
         <f>+D170+1</f>
         <v>3</v>
       </c>
-      <c r="E171" s="234" t="s">
+      <c r="E171" s="233" t="s">
         <v>201</v>
       </c>
       <c r="F171" s="213">
@@ -8586,7 +8573,7 @@
         <f>+D171+1</f>
         <v>4</v>
       </c>
-      <c r="E172" s="234" t="s">
+      <c r="E172" s="233" t="s">
         <v>202</v>
       </c>
       <c r="F172" s="213">
@@ -8606,7 +8593,7 @@
         <f>+D172+1</f>
         <v>5</v>
       </c>
-      <c r="E173" s="234" t="s">
+      <c r="E173" s="233" t="s">
         <v>203</v>
       </c>
       <c r="F173" s="213">
@@ -8626,7 +8613,7 @@
         <f>+D173+1</f>
         <v>6</v>
       </c>
-      <c r="E174" s="234" t="s">
+      <c r="E174" s="233" t="s">
         <v>204</v>
       </c>
       <c r="F174" s="213">
@@ -8636,7 +8623,7 @@
       <c r="G174" s="213">
         <v>55.13</v>
       </c>
-      <c r="H174" s="234" t="s">
+      <c r="H174" s="233" t="s">
         <v>205</v>
       </c>
       <c r="I174" s="4"/>
@@ -8664,7 +8651,7 @@
       <c r="D176" s="4">
         <v>1</v>
       </c>
-      <c r="E176" s="237" t="s">
+      <c r="E176" s="236" t="s">
         <v>211</v>
       </c>
       <c r="F176" s="213">
@@ -8685,7 +8672,7 @@
         <f t="shared" ref="D177:D182" si="14">+D176+1</f>
         <v>2</v>
       </c>
-      <c r="E177" s="237" t="s">
+      <c r="E177" s="236" t="s">
         <v>212</v>
       </c>
       <c r="F177" s="213">
@@ -8705,7 +8692,7 @@
         <f t="shared" si="14"/>
         <v>3</v>
       </c>
-      <c r="E178" s="237" t="s">
+      <c r="E178" s="236" t="s">
         <v>213</v>
       </c>
       <c r="F178" s="213">
@@ -8725,7 +8712,7 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="E179" s="237" t="s">
+      <c r="E179" s="236" t="s">
         <v>214</v>
       </c>
       <c r="F179" s="213">
@@ -8745,7 +8732,7 @@
         <f t="shared" si="14"/>
         <v>5</v>
       </c>
-      <c r="E180" s="237" t="s">
+      <c r="E180" s="236" t="s">
         <v>215</v>
       </c>
       <c r="F180" s="213">
@@ -8765,7 +8752,7 @@
         <f t="shared" si="14"/>
         <v>6</v>
       </c>
-      <c r="E181" s="237" t="s">
+      <c r="E181" s="236" t="s">
         <v>216</v>
       </c>
       <c r="F181" s="213">
@@ -8785,7 +8772,7 @@
         <f t="shared" si="14"/>
         <v>7</v>
       </c>
-      <c r="E182" s="237" t="s">
+      <c r="E182" s="236" t="s">
         <v>217</v>
       </c>
       <c r="F182" s="213">
@@ -8821,7 +8808,7 @@
       <c r="D184" s="4">
         <v>1</v>
       </c>
-      <c r="E184" s="238" t="s">
+      <c r="E184" s="237" t="s">
         <v>219</v>
       </c>
       <c r="F184" s="213">
@@ -8842,7 +8829,7 @@
         <f>+D184+1</f>
         <v>2</v>
       </c>
-      <c r="E185" s="238" t="s">
+      <c r="E185" s="237" t="s">
         <v>220</v>
       </c>
       <c r="F185" s="213">
@@ -8862,7 +8849,7 @@
         <f>+D185+1</f>
         <v>3</v>
       </c>
-      <c r="E186" s="238" t="s">
+      <c r="E186" s="237" t="s">
         <v>221</v>
       </c>
       <c r="F186" s="213">
@@ -8880,7 +8867,7 @@
         <f>+D186+1</f>
         <v>4</v>
       </c>
-      <c r="E187" s="238" t="s">
+      <c r="E187" s="237" t="s">
         <v>222</v>
       </c>
       <c r="F187" s="213">
@@ -8895,7 +8882,7 @@
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
-      <c r="E188" s="238"/>
+      <c r="E188" s="237"/>
       <c r="F188" s="213"/>
       <c r="G188" s="213"/>
       <c r="H188" s="4"/>
@@ -15226,7 +15213,7 @@
         <v>33.03</v>
       </c>
       <c r="H20" s="68"/>
-      <c r="I20" s="240" t="s">
+      <c r="I20" s="239" t="s">
         <v>1014</v>
       </c>
     </row>
@@ -17792,7 +17779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+    <sheetView topLeftCell="A151" workbookViewId="0">
       <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
@@ -17927,7 +17914,7 @@
       <c r="H6" s="88" t="s">
         <v>571</v>
       </c>
-      <c r="I6" s="241" t="s">
+      <c r="I6" s="240" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18031,7 +18018,7 @@
       <c r="H11" s="94" t="s">
         <v>578</v>
       </c>
-      <c r="I11" s="241" t="s">
+      <c r="I11" s="240" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18115,7 +18102,7 @@
       <c r="H15" s="94" t="s">
         <v>582</v>
       </c>
-      <c r="I15" s="242" t="s">
+      <c r="I15" s="241" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18256,7 +18243,7 @@
         <v>11.36</v>
       </c>
       <c r="H22" s="88"/>
-      <c r="I22" s="243" t="s">
+      <c r="I22" s="242" t="s">
         <v>588</v>
       </c>
     </row>
@@ -18281,7 +18268,7 @@
       <c r="H23" s="97" t="s">
         <v>152</v>
       </c>
-      <c r="I23" s="243" t="s">
+      <c r="I23" s="242" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18303,7 +18290,7 @@
         <v>54.14</v>
       </c>
       <c r="H24" s="88"/>
-      <c r="I24" s="244" t="s">
+      <c r="I24" s="243" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18341,7 +18328,7 @@
         <v>27.26</v>
       </c>
       <c r="H26" s="88"/>
-      <c r="I26" s="243" t="s">
+      <c r="I26" s="242" t="s">
         <v>593</v>
       </c>
     </row>
@@ -18363,7 +18350,7 @@
       <c r="G27" s="88">
         <v>49.08</v>
       </c>
-      <c r="H27" s="244" t="s">
+      <c r="H27" s="243" t="s">
         <v>865</v>
       </c>
       <c r="I27" s="88"/>
@@ -18389,7 +18376,7 @@
       <c r="H28" s="99" t="s">
         <v>597</v>
       </c>
-      <c r="I28" s="245" t="s">
+      <c r="I28" s="244" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18449,7 +18436,7 @@
       <c r="G31" s="88">
         <v>32.54</v>
       </c>
-      <c r="H31" s="245" t="s">
+      <c r="H31" s="244" t="s">
         <v>865</v>
       </c>
       <c r="I31" s="88"/>
@@ -18493,7 +18480,7 @@
       <c r="G33" s="88">
         <v>54.26</v>
       </c>
-      <c r="H33" s="245" t="s">
+      <c r="H33" s="244" t="s">
         <v>865</v>
       </c>
       <c r="I33" s="88"/>
@@ -18599,7 +18586,7 @@
       <c r="H38" s="101" t="s">
         <v>609</v>
       </c>
-      <c r="I38" s="246" t="s">
+      <c r="I38" s="245" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18683,7 +18670,7 @@
       <c r="H42" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="I42" s="247" t="s">
+      <c r="I42" s="246" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18728,7 +18715,7 @@
       <c r="H44" s="103" t="s">
         <v>615</v>
       </c>
-      <c r="I44" s="248" t="s">
+      <c r="I44" s="247" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18833,7 +18820,7 @@
       <c r="H49" s="103" t="s">
         <v>619</v>
       </c>
-      <c r="I49" s="249" t="s">
+      <c r="I49" s="248" t="s">
         <v>865</v>
       </c>
     </row>
@@ -18935,7 +18922,7 @@
       <c r="G54" s="88">
         <v>55.56</v>
       </c>
-      <c r="H54" s="249" t="s">
+      <c r="H54" s="248" t="s">
         <v>865</v>
       </c>
       <c r="I54" s="88"/>
@@ -19038,7 +19025,7 @@
       <c r="G59" s="88">
         <v>36.409999999999997</v>
       </c>
-      <c r="H59" s="249" t="s">
+      <c r="H59" s="248" t="s">
         <v>865</v>
       </c>
       <c r="I59" s="88"/>
@@ -19082,7 +19069,7 @@
       <c r="G61" s="88">
         <v>59.08</v>
       </c>
-      <c r="H61" s="250" t="s">
+      <c r="H61" s="249" t="s">
         <v>865</v>
       </c>
       <c r="I61" s="88"/>
@@ -19188,7 +19175,7 @@
       <c r="H66" s="107" t="s">
         <v>638</v>
       </c>
-      <c r="I66" s="251" t="s">
+      <c r="I66" s="250" t="s">
         <v>865</v>
       </c>
     </row>
@@ -19293,7 +19280,7 @@
       <c r="H71" s="109" t="s">
         <v>642</v>
       </c>
-      <c r="I71" s="252" t="s">
+      <c r="I71" s="251" t="s">
         <v>865</v>
       </c>
     </row>
@@ -19395,7 +19382,7 @@
       <c r="G76" s="93">
         <v>55.05</v>
       </c>
-      <c r="H76" s="253" t="s">
+      <c r="H76" s="252" t="s">
         <v>865</v>
       </c>
       <c r="I76" s="88"/>
@@ -19501,7 +19488,7 @@
       <c r="H81" s="110" t="s">
         <v>652</v>
       </c>
-      <c r="I81" s="254" t="s">
+      <c r="I81" s="253" t="s">
         <v>865</v>
       </c>
     </row>
@@ -19624,7 +19611,7 @@
       <c r="G87" s="88">
         <v>56.54</v>
       </c>
-      <c r="H87" s="255" t="s">
+      <c r="H87" s="254" t="s">
         <v>865</v>
       </c>
       <c r="I87" s="88"/>
@@ -19853,7 +19840,7 @@
       <c r="G98" s="88">
         <v>56.17</v>
       </c>
-      <c r="H98" s="256" t="s">
+      <c r="H98" s="255" t="s">
         <v>865</v>
       </c>
       <c r="I98" s="88"/>
@@ -19998,7 +19985,7 @@
       <c r="G105" s="93">
         <v>12.51</v>
       </c>
-      <c r="H105" s="257" t="s">
+      <c r="H105" s="256" t="s">
         <v>865</v>
       </c>
       <c r="I105" s="88"/>
@@ -20087,7 +20074,7 @@
       <c r="H109" s="114" t="s">
         <v>683</v>
       </c>
-      <c r="I109" s="257" t="s">
+      <c r="I109" s="256" t="s">
         <v>865</v>
       </c>
     </row>
@@ -20213,7 +20200,7 @@
       <c r="H115" s="114" t="s">
         <v>688</v>
       </c>
-      <c r="I115" s="258" t="s">
+      <c r="I115" s="257" t="s">
         <v>865</v>
       </c>
     </row>
@@ -20294,7 +20281,7 @@
       <c r="G119" s="88">
         <v>35.32</v>
       </c>
-      <c r="H119" s="259" t="s">
+      <c r="H119" s="258" t="s">
         <v>865</v>
       </c>
       <c r="I119" s="88"/>
@@ -20506,7 +20493,7 @@
       <c r="G129" s="88">
         <v>55.55</v>
       </c>
-      <c r="H129" s="260" t="s">
+      <c r="H129" s="259" t="s">
         <v>865</v>
       </c>
       <c r="I129" s="88"/>
@@ -20675,7 +20662,7 @@
       <c r="H137" s="117" t="s">
         <v>716</v>
       </c>
-      <c r="I137" s="261" t="s">
+      <c r="I137" s="260" t="s">
         <v>865</v>
       </c>
     </row>
@@ -20798,7 +20785,7 @@
       <c r="G143" s="93">
         <v>55.42</v>
       </c>
-      <c r="H143" s="262" t="s">
+      <c r="H143" s="261" t="s">
         <v>865</v>
       </c>
       <c r="I143" s="88"/>
@@ -21195,7 +21182,7 @@
       <c r="G162" s="88">
         <v>58.49</v>
       </c>
-      <c r="H162" s="263" t="s">
+      <c r="H162" s="262" t="s">
         <v>865</v>
       </c>
       <c r="I162" s="88"/>

</xml_diff>

<commit_message>
TS 2.4 2.5 Padam templates review
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5D698-B868-4FB2-ABAA-A982772AABB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E6A2CC-C9E9-494F-ACC7-4368D031FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -4975,7 +4975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
@@ -9771,8 +9771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J105" sqref="J105"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 2.4 Ghanam Corrections
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E6A2CC-C9E9-494F-ACC7-4368D031FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E4818E-97BF-4AD4-96E0-62047C3B7FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9771,8 +9771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="C67" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12664,8 +12664,11 @@
       <c r="J133" s="30"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J80" r:id="rId1" xr:uid="{04C9970A-919A-47CF-AEE8-A0ED76966188}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 6.1 TTD first hearing - 20/09/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647CF100-436E-4743-BC69-AF1247463788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76B47CE-75D9-4593-A8AD-0B6DD920B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -3085,13 +3085,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="195" x14ac:knownFonts="1">
+  <fonts count="197" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4302,70 +4314,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="192" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="194" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="192" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="194" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="192" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="194" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="186" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="183" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="186" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="181" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="175" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="174" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="173" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="172" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="168" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="168" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="165" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="163" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="193" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="195" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="193" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="193" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="195" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="195" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="158" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="196" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="156" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="158" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4373,18 +4387,18 @@
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="147" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="142" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4398,19 +4412,19 @@
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="126" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="192" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="194" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4426,30 +4440,30 @@
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="96" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4462,152 +4476,152 @@
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="133" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="130" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="129" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="128" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="196" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="196" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="196" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="191" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4630,8 +4644,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12673,8 +12687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17779,7 +17793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A157" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -22021,8 +22035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22033,7 +22047,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52" customWidth="1"/>
+    <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22166,7 +22180,9 @@
       <c r="H6" s="124" t="s">
         <v>745</v>
       </c>
-      <c r="I6" s="120"/>
+      <c r="I6" s="253" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="120"/>
@@ -22227,7 +22243,9 @@
       <c r="H9" s="124" t="s">
         <v>751</v>
       </c>
-      <c r="I9" s="120"/>
+      <c r="I9" s="254" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="120"/>
@@ -24147,8 +24165,11 @@
       <c r="J105" s="141"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{6974D439-E431-4D0C-905C-CF0D14AEA60F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 6.2 Jatai hearing template and TTD Jatai Excel - 23/09/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A301FFD9-98CD-4621-AB4A-CC824D7318C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2146DC54-B59E-4138-B11A-91A94F14A792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -3085,13 +3085,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="197" x14ac:knownFonts="1">
+  <fonts count="198" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4314,70 +4320,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="194" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="195" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="194" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="195" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="194" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="195" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="186" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="183" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="186" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="176" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="175" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="175" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="174" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="171" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="171" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="170" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="166" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="165" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="161" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="195" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="196" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="195" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="195" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="158" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="196" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="196" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="196" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="158" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4386,17 +4393,17 @@
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="150" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="148" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="144" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4411,18 +4418,18 @@
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="194" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="195" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="127" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4439,29 +4446,29 @@
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="98" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4475,45 +4482,45 @@
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="70" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4521,105 +4528,105 @@
     <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="134" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="132" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="133" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="130" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="196" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="196" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="196" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="197" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="197" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="193" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4643,7 +4650,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -22035,8 +22042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22513,7 +22520,9 @@
         <v>59.35</v>
       </c>
       <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
+      <c r="I22" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="120"/>
@@ -22595,7 +22604,9 @@
       <c r="H26" s="129" t="s">
         <v>770</v>
       </c>
-      <c r="I26" s="120"/>
+      <c r="I26" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="120"/>
@@ -24174,9 +24185,10 @@
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{6974D439-E431-4D0C-905C-CF0D14AEA60F}"/>
     <hyperlink ref="I11" r:id="rId2" xr:uid="{550E0FD9-A856-4D53-A16E-FE9EAADA2726}"/>
+    <hyperlink ref="I24" r:id="rId3" xr:uid="{90E16496-E5DD-4499-A0C4-AC1E699C075C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 3.2 Ghanam Tamil - 25/09/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1965FB5F-0055-4199-8F1D-D900CC9F8826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E7DAE7-8505-4AD5-B56E-35D51C7E3A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -22042,8 +22042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22875,7 +22875,9 @@
         <v>26.4</v>
       </c>
       <c r="H39" s="120"/>
-      <c r="I39" s="120"/>
+      <c r="I39" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="120"/>
@@ -24200,7 +24202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TS 3.4 Jatai Ghanam formatting  Final - 08/10/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B48E39A-F816-46B1-AC91-F4A81AEFAD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B218C8F8-0CD1-4E6F-A362-654CECBDE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12694,8 +12694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14802,8 +14802,11 @@
       <c r="I99" s="63"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I65" r:id="rId1" xr:uid="{C7884D16-66DF-4728-A49B-5C170AAB79E8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 4.3 & TS 4.4 Baraha Inputs from Raja
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B218C8F8-0CD1-4E6F-A362-654CECBDE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C12BF4-4FD7-4442-A744-908B64ABD27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -12694,7 +12694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
@@ -22045,7 +22045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TS Padam Template 4.6, 6.3 to 6.6 - 10/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C12BF4-4FD7-4442-A744-908B64ABD27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7320B65-A3CF-4CA9-8D8F-28AC3EE7D4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -4320,7 +4320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4653,6 +4653,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="79" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12683,7 +12684,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J80" r:id="rId1" xr:uid="{04C9970A-919A-47CF-AEE8-A0ED76966188}"/>
+    <hyperlink ref="J80" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -14803,7 +14804,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I65" r:id="rId1" xr:uid="{C7884D16-66DF-4728-A49B-5C170AAB79E8}"/>
+    <hyperlink ref="I65" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
@@ -22027,14 +22028,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{F98ED066-CB19-4B46-8CC6-0978F01090BC}"/>
-    <hyperlink ref="I8" r:id="rId2" xr:uid="{7A24F6C1-A105-4B74-A527-D47A71FE5DCB}"/>
-    <hyperlink ref="I13" r:id="rId3" xr:uid="{24E77FE3-7C84-4E8F-849A-A8579B12B0B4}"/>
-    <hyperlink ref="I17" r:id="rId4" xr:uid="{6DCA4BCF-B88C-468C-88BF-CF86647D06D4}"/>
-    <hyperlink ref="I26" r:id="rId5" xr:uid="{F617508C-F774-45DB-9E28-079ED15C8C13}"/>
-    <hyperlink ref="I30" r:id="rId6" xr:uid="{59834FBE-AB23-4410-9105-7B00D3E26EF4}"/>
-    <hyperlink ref="I35" r:id="rId7" xr:uid="{BC04F59C-EDA4-48D1-A032-AECB8D743EEC}"/>
-    <hyperlink ref="I40" r:id="rId8" xr:uid="{A6DC3357-ACE3-4587-9136-EA5B178532BC}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="I13" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="I17" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="I26" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="I30" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="I35" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="I40" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
@@ -22045,8 +22046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22924,7 +22925,9 @@
       <c r="H41" s="134" t="s">
         <v>790</v>
       </c>
-      <c r="I41" s="120"/>
+      <c r="I41" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="120"/>
@@ -23006,7 +23009,9 @@
       <c r="H45" s="134" t="s">
         <v>794</v>
       </c>
-      <c r="I45" s="120"/>
+      <c r="I45" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="120"/>
@@ -23115,7 +23120,9 @@
       <c r="H51" s="135" t="s">
         <v>802</v>
       </c>
-      <c r="I51" s="120"/>
+      <c r="I51" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="120"/>
@@ -23216,7 +23223,9 @@
         <v>809</v>
       </c>
       <c r="H56" s="120"/>
-      <c r="I56" s="120"/>
+      <c r="I56" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="120"/>
@@ -23319,7 +23328,9 @@
       <c r="H61" s="138" t="s">
         <v>814</v>
       </c>
-      <c r="I61" s="120"/>
+      <c r="I61" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="120"/>
@@ -23399,7 +23410,9 @@
         <v>51.1</v>
       </c>
       <c r="H65" s="120"/>
-      <c r="I65" s="120"/>
+      <c r="I65" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="120"/>
@@ -23502,7 +23515,9 @@
       <c r="H70" s="139" t="s">
         <v>825</v>
       </c>
-      <c r="I70" s="120"/>
+      <c r="I70" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="120"/>
@@ -23561,7 +23576,9 @@
         <v>22.18</v>
       </c>
       <c r="H73" s="120"/>
-      <c r="I73" s="120"/>
+      <c r="I73" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="120"/>
@@ -23624,7 +23641,9 @@
         <v>57.55</v>
       </c>
       <c r="H76" s="120"/>
-      <c r="I76" s="120"/>
+      <c r="I76" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="120"/>
@@ -23644,7 +23663,9 @@
       <c r="B78" s="121">
         <v>44143</v>
       </c>
-      <c r="C78" s="120"/>
+      <c r="C78" s="120">
+        <v>54.48</v>
+      </c>
       <c r="D78" s="126">
         <v>1</v>
       </c>
@@ -23723,7 +23744,9 @@
         <v>54.09</v>
       </c>
       <c r="H81" s="120"/>
-      <c r="I81" s="120"/>
+      <c r="I81" s="255" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="120"/>
@@ -23822,6 +23845,9 @@
       </c>
       <c r="H86" s="140" t="s">
         <v>841</v>
+      </c>
+      <c r="I86" s="255" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -23852,10 +23878,10 @@
       <c r="E88" s="141" t="s">
         <v>842</v>
       </c>
-      <c r="F88" s="141">
+      <c r="F88" s="256">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G88" s="141">
+      <c r="G88" s="256">
         <v>8.32</v>
       </c>
       <c r="H88" s="141"/>
@@ -23905,7 +23931,9 @@
         <v>29.26</v>
       </c>
       <c r="H90" s="141"/>
-      <c r="I90" s="141"/>
+      <c r="I90" s="255" t="s">
+        <v>865</v>
+      </c>
       <c r="J90" s="141"/>
     </row>
     <row r="91" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -23967,7 +23995,9 @@
         <v>40.520000000000003</v>
       </c>
       <c r="H93" s="141"/>
-      <c r="I93" s="141"/>
+      <c r="I93" s="255" t="s">
+        <v>865</v>
+      </c>
       <c r="J93" s="141"/>
     </row>
     <row r="94" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -24095,7 +24125,9 @@
         <v>43.29</v>
       </c>
       <c r="H99" s="141"/>
-      <c r="I99" s="141"/>
+      <c r="I99" s="255" t="s">
+        <v>865</v>
+      </c>
       <c r="J99" s="141"/>
     </row>
     <row r="100" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -24139,7 +24171,9 @@
         <v>860</v>
       </c>
       <c r="H101" s="141"/>
-      <c r="I101" s="141"/>
+      <c r="I101" s="255" t="s">
+        <v>865</v>
+      </c>
       <c r="J101" s="141"/>
     </row>
     <row r="102" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -24192,12 +24226,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{6974D439-E431-4D0C-905C-CF0D14AEA60F}"/>
-    <hyperlink ref="I11" r:id="rId2" xr:uid="{550E0FD9-A856-4D53-A16E-FE9EAADA2726}"/>
-    <hyperlink ref="I24" r:id="rId3" xr:uid="{90E16496-E5DD-4499-A0C4-AC1E699C075C}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="I11" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="I24" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="I53" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="I58" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="I63" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="I67" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="I78" r:id="rId8" xr:uid="{4003FB2D-1513-462C-8D06-0A0A7D48F1BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 7.1 Padam Template TTD listening - 23/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7320B65-A3CF-4CA9-8D8F-28AC3EE7D4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2320D5F-1216-4483-BDD3-5B7758E3267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -17,21 +17,11 @@
     <sheet name="Kandam7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -3085,13 +3075,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="198" x14ac:knownFonts="1">
+  <fonts count="199" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4320,70 +4316,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="195" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="196" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="195" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="196" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="195" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="196" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="186" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="185" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="184" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="184" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="188" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="187" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="182" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="181" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="180" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="177" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="177" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="176" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="176" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="175" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="174" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="172" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="172" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="171" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="171" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="170" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="168" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="167" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="167" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="166" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="166" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="163" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="162" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="196" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="197" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="196" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="196" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="197" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="197" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="160" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="198" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="159" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="160" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4392,17 +4389,17 @@
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="151" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="150" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="150" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="149" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="146" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="145" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4417,18 +4414,18 @@
     <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="130" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="195" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="196" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="129" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="128" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4445,29 +4442,29 @@
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="101" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="100" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="99" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4481,45 +4478,45 @@
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="80" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="78" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="72" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="71" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="52" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4527,105 +4524,105 @@
     <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="135" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="133" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="132" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="134" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="132" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="197" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="197" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="198" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="198" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="198" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="194" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="188" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="193" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="187" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4649,11 +4646,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="79" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22046,7 +22043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
@@ -24244,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24418,7 +24415,9 @@
         <v>49.51</v>
       </c>
       <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
+      <c r="I7" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="143"/>

</xml_diff>

<commit_message>
nmv 06 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2320D5F-1216-4483-BDD3-5B7758E3267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF17002-266A-4FFA-A6E3-E4F914AAB795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4651,6 +4651,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4991,10 +4994,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7327,7 +7330,7 @@
         <v>16.07</v>
       </c>
       <c r="H108" s="4"/>
-      <c r="I108" s="4" t="s">
+      <c r="I108" s="258" t="s">
         <v>124</v>
       </c>
     </row>
@@ -9779,7 +9782,7 @@
     <hyperlink ref="I7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24241,7 +24244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 12 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF17002-266A-4FFA-A6E3-E4F914AAB795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109CAEB9-7366-4C1C-9337-BBDE0ACD511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4316,7 +4316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4651,9 +4651,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="197" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7330,7 +7327,7 @@
         <v>16.07</v>
       </c>
       <c r="H108" s="4"/>
-      <c r="I108" s="258" t="s">
+      <c r="I108" s="51" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update TTD JatA PaaraayaNam-Jatai.xlsx
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109CAEB9-7366-4C1C-9337-BBDE0ACD511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7215C3A-E07B-47F8-BA29-8932D810F64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -4992,7 +4992,7 @@
   <dimension ref="A4:M275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="I108" sqref="I108"/>
     </sheetView>
@@ -24242,7 +24242,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24476,7 +24476,9 @@
         <v>47.5</v>
       </c>
       <c r="H10" s="143"/>
-      <c r="I10" s="143"/>
+      <c r="I10" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="143"/>
@@ -24598,7 +24600,9 @@
         <v>45.29</v>
       </c>
       <c r="H16" s="143"/>
-      <c r="I16" s="143"/>
+      <c r="I16" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="143"/>
@@ -24804,7 +24808,9 @@
         <v>45.13</v>
       </c>
       <c r="H26" s="143"/>
-      <c r="I26" s="143"/>
+      <c r="I26" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="143"/>
@@ -24905,7 +24911,9 @@
         <v>48.05</v>
       </c>
       <c r="H31" s="143"/>
-      <c r="I31" s="143"/>
+      <c r="I31" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="143"/>

</xml_diff>

<commit_message>
TS 7.2 7.3 Padam XLs listening - 07/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7215C3A-E07B-47F8-BA29-8932D810F64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9A88B8-02C2-41CF-A848-94D7BFE31B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -4991,7 +4991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="I108" sqref="I108"/>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25005,7 +25005,9 @@
       <c r="H36" s="154" t="s">
         <v>902</v>
       </c>
-      <c r="I36" s="143"/>
+      <c r="I36" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="143"/>
@@ -25088,7 +25090,9 @@
       <c r="H40" s="154" t="s">
         <v>903</v>
       </c>
-      <c r="I40" s="143"/>
+      <c r="I40" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="143"/>
@@ -25358,7 +25362,6 @@
         <v>45.4</v>
       </c>
       <c r="H53" s="143"/>
-      <c r="I53" s="143"/>
     </row>
     <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="143"/>
@@ -25381,7 +25384,9 @@
       <c r="H54" s="155" t="s">
         <v>916</v>
       </c>
-      <c r="I54" s="143"/>
+      <c r="I54" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="143"/>
@@ -27299,7 +27304,11 @@
       <c r="I152" s="166"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I34" r:id="rId1" xr:uid="{F86DE5FB-8C78-403E-820F-E07CF9AE26A9}"/>
+    <hyperlink ref="I38" r:id="rId2" xr:uid="{9E5DB6B5-1C4F-4185-9EF1-DC506AA73F77}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TS 7.3 Jatai listening - 09/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAE367A-0CCC-4BAA-B469-704257C85F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05AB83F-5519-4A9A-946B-CC671C2E9E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25646,7 +25646,9 @@
       <c r="H67" s="157" t="s">
         <v>931</v>
       </c>
-      <c r="I67" s="143"/>
+      <c r="I67" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="143"/>
@@ -25790,7 +25792,9 @@
         <v>42.33</v>
       </c>
       <c r="H74" s="143"/>
-      <c r="I74" s="143"/>
+      <c r="I74" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="143"/>

</xml_diff>

<commit_message>
TS 7.3 Template hearing TTD - 10/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05AB83F-5519-4A9A-946B-CC671C2E9E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A48D966-109A-4F47-AF88-FB3E3F169A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -17801,7 +17801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
+    <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25938,7 +25938,9 @@
         <v>33.19</v>
       </c>
       <c r="H81" s="143"/>
-      <c r="I81" s="143"/>
+      <c r="I81" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="143"/>

</xml_diff>

<commit_message>
TS 7.4 Template Jatai listening - 13/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A48D966-109A-4F47-AF88-FB3E3F169A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8EE796-D004-4F62-AD28-09F943EA2285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26021,7 +26021,9 @@
         <v>40.35</v>
       </c>
       <c r="H85" s="143"/>
-      <c r="I85" s="143"/>
+      <c r="I85" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="143"/>
@@ -26083,7 +26085,9 @@
       <c r="H88" s="160" t="s">
         <v>951</v>
       </c>
-      <c r="I88" s="143"/>
+      <c r="I88" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="143"/>
@@ -26143,7 +26147,6 @@
         <v>26.14</v>
       </c>
       <c r="H91" s="143"/>
-      <c r="I91" s="143"/>
     </row>
     <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="143"/>
@@ -26187,7 +26190,9 @@
       <c r="H93" s="162" t="s">
         <v>960</v>
       </c>
-      <c r="I93" s="143"/>
+      <c r="I93" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="143"/>

</xml_diff>

<commit_message>
TS 7.5 Jata Listening - 27/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DC3BF8-07C9-445D-BE7C-68DB9E3030B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF80601F-F43C-4A1E-80E3-06DA252C229C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I111" sqref="I111"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26649,7 +26649,9 @@
         <v>39.049999999999997</v>
       </c>
       <c r="H115" s="143"/>
-      <c r="I115" s="143"/>
+      <c r="I115" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="143"/>

</xml_diff>

<commit_message>
TS 7.5 Padam Jatai listening - 29/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF80601F-F43C-4A1E-80E3-06DA252C229C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B88F5-301E-40F0-B2E5-9B7084A7E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -24242,7 +24242,7 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="I115" sqref="I115"/>
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26753,7 +26753,9 @@
         <v>39.520000000000003</v>
       </c>
       <c r="H120" s="143"/>
-      <c r="I120" s="143"/>
+      <c r="I120" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="143"/>
@@ -26813,7 +26815,9 @@
         <v>39.44</v>
       </c>
       <c r="H123" s="143"/>
-      <c r="I123" s="143"/>
+      <c r="I123" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="143"/>
@@ -26915,7 +26919,9 @@
         <v>44.1</v>
       </c>
       <c r="H128" s="166"/>
-      <c r="I128" s="166"/>
+      <c r="I128" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="166"/>

</xml_diff>

<commit_message>
TS 7.5 Padam Jatai listening - 07/04/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B88F5-301E-40F0-B2E5-9B7084A7E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347C36D7-0FC9-4CCA-9580-FAE2374C4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="1016">
   <si>
     <t>Date</t>
   </si>
@@ -24241,8 +24241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27086,7 +27086,9 @@
         <v>46.06</v>
       </c>
       <c r="H136" s="166"/>
-      <c r="I136" s="166"/>
+      <c r="I136" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="166"/>
@@ -27230,7 +27232,9 @@
         <v>34.17</v>
       </c>
       <c r="H143" s="166"/>
-      <c r="I143" s="166"/>
+      <c r="I143" s="257" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="166"/>

</xml_diff>

<commit_message>
nmv 23 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347C36D7-0FC9-4CCA-9580-FAE2374C4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD705BE-2AE7-4D41-B415-7958668CD3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -9787,8 +9787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView topLeftCell="C67" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24241,7 +24241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 06 09 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271BF671-33B3-4E91-9A7B-156CB46697AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52E6A7-B177-40B2-80FE-1E2BE3211352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9753,8 +9753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 13 12 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52E6A7-B177-40B2-80FE-1E2BE3211352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9DC27B-9FB7-4D29-990B-8570BAAB04F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="195" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="195" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4651,6 +4651,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9753,7 +9754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
@@ -12658,8 +12659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14220,7 +14221,7 @@
         <v>20.57</v>
       </c>
       <c r="H65" s="63"/>
-      <c r="I65" s="63" t="s">
+      <c r="I65" s="258" t="s">
         <v>433</v>
       </c>
     </row>
@@ -14766,11 +14767,8 @@
       <c r="I99" s="63"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I65" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
nmv 08 04 2025
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9DC27B-9FB7-4D29-990B-8570BAAB04F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D88EFE-DB94-4306-8DA7-95DBB0320793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Kandam6" sheetId="6" r:id="rId6"/>
     <sheet name="Kandam7" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -2180,9 +2180,6 @@
     <t>5.7.5.1</t>
   </si>
   <si>
-    <t>5.7.61</t>
-  </si>
-  <si>
     <t>5.7.7.1</t>
   </si>
   <si>
@@ -3069,6 +3066,9 @@
   </si>
   <si>
     <t>H1 and H2</t>
+  </si>
+  <si>
+    <t>5.7.6.1</t>
   </si>
 </sst>
 </file>
@@ -4651,7 +4651,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="80" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5778,7 +5780,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="208" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F39" s="203">
         <f>+G38</f>
@@ -7257,7 +7259,7 @@
         <v>47.51</v>
       </c>
       <c r="H106" s="211" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I106" s="4"/>
     </row>
@@ -7453,7 +7455,7 @@
         <v>55.39</v>
       </c>
       <c r="H116" s="213" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I116" s="4"/>
     </row>
@@ -7590,7 +7592,7 @@
         <v>5.59</v>
       </c>
       <c r="H123" s="212" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I123" s="4" t="s">
         <v>164</v>
@@ -7675,7 +7677,7 @@
         <v>56.45</v>
       </c>
       <c r="H127" s="217" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I127" s="4"/>
     </row>
@@ -7795,7 +7797,7 @@
         <v>59.01</v>
       </c>
       <c r="H133" s="219" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I133" s="4"/>
     </row>
@@ -7932,7 +7934,7 @@
         <v>26.55</v>
       </c>
       <c r="H140" s="220" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I140" s="4"/>
     </row>
@@ -8035,7 +8037,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B146" s="221" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C146" s="4"/>
       <c r="D146" s="4">
@@ -8153,7 +8155,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B152" s="223" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="4">
@@ -8346,7 +8348,7 @@
         <v>15.05</v>
       </c>
       <c r="H161" s="224" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I161" s="4" t="s">
         <v>190</v>
@@ -9904,7 +9906,7 @@
         <v>226</v>
       </c>
       <c r="I6" s="171" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -9993,7 +9995,7 @@
         <v>231</v>
       </c>
       <c r="I10" s="170" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -10081,7 +10083,7 @@
         <v>238</v>
       </c>
       <c r="I14" s="170" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J14" s="1"/>
     </row>
@@ -10213,7 +10215,7 @@
         <v>245</v>
       </c>
       <c r="I20" s="172" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J20" s="14" t="s">
         <v>246</v>
@@ -10257,7 +10259,7 @@
         <v>152</v>
       </c>
       <c r="I22" s="173" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>247</v>
@@ -10306,7 +10308,7 @@
         <v>250</v>
       </c>
       <c r="I24" s="174" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J24" s="1"/>
     </row>
@@ -10417,7 +10419,7 @@
         <v>255</v>
       </c>
       <c r="I29" s="174" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J29" s="10"/>
     </row>
@@ -10506,7 +10508,7 @@
         <v>260</v>
       </c>
       <c r="I33" s="175" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J33" s="10"/>
     </row>
@@ -10606,7 +10608,7 @@
         <v>266</v>
       </c>
       <c r="I38" s="176" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J38" s="10"/>
     </row>
@@ -10694,7 +10696,7 @@
         <v>269</v>
       </c>
       <c r="I42" s="177" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J42" s="10"/>
     </row>
@@ -10760,7 +10762,7 @@
         <v>152</v>
       </c>
       <c r="I45" s="178" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J45" s="10"/>
     </row>
@@ -10807,7 +10809,7 @@
         <v>278</v>
       </c>
       <c r="I47" s="179" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J47" s="10"/>
     </row>
@@ -10917,7 +10919,7 @@
         <v>282</v>
       </c>
       <c r="I52" s="180" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J52" s="10"/>
     </row>
@@ -11071,7 +11073,7 @@
         <v>292</v>
       </c>
       <c r="I59" s="181" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J59" s="10"/>
     </row>
@@ -11216,7 +11218,7 @@
         <v>299</v>
       </c>
       <c r="I66" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J66" s="10"/>
     </row>
@@ -11325,7 +11327,7 @@
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J71" s="10"/>
     </row>
@@ -11477,7 +11479,7 @@
       </c>
       <c r="H78" s="10"/>
       <c r="I78" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J78" s="10"/>
     </row>
@@ -11566,7 +11568,7 @@
         <v>317</v>
       </c>
       <c r="I82" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J82" s="10"/>
     </row>
@@ -11666,7 +11668,7 @@
         <v>323</v>
       </c>
       <c r="I87" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J87" s="30"/>
     </row>
@@ -11753,7 +11755,7 @@
         <v>330</v>
       </c>
       <c r="I91" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J91" s="30"/>
     </row>
@@ -11840,7 +11842,7 @@
       </c>
       <c r="H95" s="30"/>
       <c r="I95" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J95" s="30"/>
     </row>
@@ -11923,7 +11925,7 @@
         <v>338</v>
       </c>
       <c r="I99" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J99" s="30"/>
     </row>
@@ -12012,7 +12014,7 @@
         <v>343</v>
       </c>
       <c r="I103" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J103" s="30"/>
     </row>
@@ -12053,7 +12055,7 @@
       <c r="H105" s="30"/>
       <c r="I105" s="30"/>
       <c r="J105" s="30" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -12123,7 +12125,7 @@
         <v>348</v>
       </c>
       <c r="I108" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J108" s="30"/>
     </row>
@@ -12211,7 +12213,7 @@
         <v>353</v>
       </c>
       <c r="I112" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J112" s="30"/>
     </row>
@@ -12321,7 +12323,7 @@
         <v>358</v>
       </c>
       <c r="I117" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J117" s="30"/>
     </row>
@@ -12345,7 +12347,7 @@
         <v>44068</v>
       </c>
       <c r="C119" s="183" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D119" s="4">
         <v>1</v>
@@ -12410,7 +12412,7 @@
         <v>363</v>
       </c>
       <c r="I121" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J121" s="30"/>
     </row>
@@ -12447,7 +12449,7 @@
       </c>
       <c r="G123" s="32"/>
       <c r="H123" s="183" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I123" s="44"/>
       <c r="J123" s="30" t="s">
@@ -12493,7 +12495,7 @@
       </c>
       <c r="H125" s="30"/>
       <c r="I125" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J125" s="30"/>
     </row>
@@ -12559,7 +12561,7 @@
         <v>152</v>
       </c>
       <c r="I128" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J128" s="30"/>
     </row>
@@ -12606,7 +12608,7 @@
         <v>372</v>
       </c>
       <c r="I130" s="182" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J130" s="30"/>
     </row>
@@ -12659,7 +12661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
@@ -12814,7 +12816,7 @@
         <v>55.04</v>
       </c>
       <c r="H7" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I7" s="30"/>
     </row>
@@ -12943,7 +12945,7 @@
         <v>54.55</v>
       </c>
       <c r="H13" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I13" s="49"/>
       <c r="J13" s="49"/>
@@ -13066,7 +13068,7 @@
         <v>56.32</v>
       </c>
       <c r="H18" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
@@ -13190,7 +13192,7 @@
         <v>58.58</v>
       </c>
       <c r="H23" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
@@ -13288,7 +13290,7 @@
         <v>58.45</v>
       </c>
       <c r="H27" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I27" s="49"/>
       <c r="J27" s="49"/>
@@ -13411,7 +13413,7 @@
         <v>57.46</v>
       </c>
       <c r="H32" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I32" s="56" t="s">
         <v>399</v>
@@ -13611,7 +13613,7 @@
         <v>53.46</v>
       </c>
       <c r="H40" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I40" s="58" t="s">
         <v>407</v>
@@ -13761,7 +13763,7 @@
         <v>57.44</v>
       </c>
       <c r="H46" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I46" s="49"/>
       <c r="J46" s="49"/>
@@ -13884,7 +13886,7 @@
         <v>33.090000000000003</v>
       </c>
       <c r="H51" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I51" s="60" t="s">
         <v>418</v>
@@ -14059,7 +14061,7 @@
         <v>57.19</v>
       </c>
       <c r="H58" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I58" s="61" t="s">
         <v>422</v>
@@ -14181,7 +14183,7 @@
         <v>54.5</v>
       </c>
       <c r="H63" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I63" s="61" t="s">
         <v>431</v>
@@ -14221,7 +14223,7 @@
         <v>20.57</v>
       </c>
       <c r="H65" s="63"/>
-      <c r="I65" s="258" t="s">
+      <c r="I65" t="s">
         <v>433</v>
       </c>
     </row>
@@ -14285,7 +14287,7 @@
         <v>56.51</v>
       </c>
       <c r="H68" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I68" s="65" t="s">
         <v>436</v>
@@ -14390,7 +14392,7 @@
         <v>56.26</v>
       </c>
       <c r="H73" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I73" s="63"/>
     </row>
@@ -14535,7 +14537,7 @@
         <v>55.12</v>
       </c>
       <c r="H80" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I80" s="63"/>
     </row>
@@ -14573,7 +14575,7 @@
         <v>21.12</v>
       </c>
       <c r="H82" s="184" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I82" s="63" t="s">
         <v>450</v>
@@ -14911,7 +14913,7 @@
         <v>455</v>
       </c>
       <c r="I6" s="185" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15037,7 +15039,7 @@
         <v>460</v>
       </c>
       <c r="I12" s="185" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15138,7 +15140,7 @@
         <v>43.54</v>
       </c>
       <c r="H17" s="186" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I17" s="68"/>
     </row>
@@ -15200,7 +15202,7 @@
       </c>
       <c r="H20" s="68"/>
       <c r="I20" s="228" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15225,7 +15227,7 @@
         <v>471</v>
       </c>
       <c r="I21" s="186" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15327,7 +15329,7 @@
         <v>54.01</v>
       </c>
       <c r="I26" s="187" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15408,7 +15410,7 @@
         <v>49.15</v>
       </c>
       <c r="H30" s="188" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I30" s="68"/>
     </row>
@@ -15511,7 +15513,7 @@
         <v>57.46</v>
       </c>
       <c r="H35" s="189" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I35" s="68"/>
     </row>
@@ -15677,7 +15679,7 @@
         <v>55.58</v>
       </c>
       <c r="H43" s="190" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I43" s="68"/>
     </row>
@@ -15804,7 +15806,7 @@
         <v>499</v>
       </c>
       <c r="I49" s="192" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -15885,7 +15887,7 @@
         <v>37.42</v>
       </c>
       <c r="H53" s="193" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I53" s="68"/>
     </row>
@@ -15967,7 +15969,7 @@
         <v>59.12</v>
       </c>
       <c r="H57" s="193" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I57" s="68"/>
     </row>
@@ -16157,7 +16159,7 @@
         <v>516</v>
       </c>
       <c r="I66" s="193" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -16468,7 +16470,7 @@
         <v>532</v>
       </c>
       <c r="I81" s="197" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -16573,7 +16575,7 @@
         <v>536</v>
       </c>
       <c r="I86" s="197" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -16657,7 +16659,7 @@
         <v>541</v>
       </c>
       <c r="I90" s="197" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -16760,7 +16762,7 @@
       </c>
       <c r="H95" s="68"/>
       <c r="I95" s="198" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -17765,8 +17767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17901,7 +17903,7 @@
         <v>571</v>
       </c>
       <c r="I6" s="229" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18005,7 +18007,7 @@
         <v>578</v>
       </c>
       <c r="I11" s="229" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18089,7 +18091,7 @@
         <v>582</v>
       </c>
       <c r="I15" s="230" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18255,7 +18257,7 @@
         <v>152</v>
       </c>
       <c r="I23" s="252" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18277,7 +18279,7 @@
       </c>
       <c r="H24" s="88"/>
       <c r="I24" s="232" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18337,7 +18339,7 @@
         <v>49.08</v>
       </c>
       <c r="H27" s="232" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I27" s="88"/>
     </row>
@@ -18363,7 +18365,7 @@
         <v>597</v>
       </c>
       <c r="I28" s="233" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18423,7 +18425,7 @@
         <v>32.54</v>
       </c>
       <c r="H31" s="233" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I31" s="88"/>
     </row>
@@ -18467,7 +18469,7 @@
         <v>54.26</v>
       </c>
       <c r="H33" s="233" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I33" s="88"/>
     </row>
@@ -18573,7 +18575,7 @@
         <v>609</v>
       </c>
       <c r="I38" s="234" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18657,7 +18659,7 @@
         <v>152</v>
       </c>
       <c r="I42" s="235" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18702,7 +18704,7 @@
         <v>615</v>
       </c>
       <c r="I44" s="236" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18807,7 +18809,7 @@
         <v>619</v>
       </c>
       <c r="I49" s="237" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -18909,7 +18911,7 @@
         <v>55.56</v>
       </c>
       <c r="H54" s="237" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I54" s="88"/>
     </row>
@@ -19012,7 +19014,7 @@
         <v>36.409999999999997</v>
       </c>
       <c r="H59" s="237" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I59" s="88"/>
     </row>
@@ -19056,7 +19058,7 @@
         <v>59.08</v>
       </c>
       <c r="H61" s="238" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I61" s="88"/>
     </row>
@@ -19162,7 +19164,7 @@
         <v>638</v>
       </c>
       <c r="I66" s="239" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -19267,7 +19269,7 @@
         <v>642</v>
       </c>
       <c r="I71" s="240" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -19369,7 +19371,7 @@
         <v>55.05</v>
       </c>
       <c r="H76" s="241" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I76" s="88"/>
     </row>
@@ -19475,7 +19477,7 @@
         <v>652</v>
       </c>
       <c r="I81" s="242" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -19598,7 +19600,7 @@
         <v>56.54</v>
       </c>
       <c r="H87" s="243" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I87" s="88"/>
     </row>
@@ -19827,7 +19829,7 @@
         <v>56.17</v>
       </c>
       <c r="H98" s="244" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I98" s="88"/>
     </row>
@@ -19972,7 +19974,7 @@
         <v>12.51</v>
       </c>
       <c r="H105" s="245" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I105" s="88"/>
     </row>
@@ -20061,7 +20063,7 @@
         <v>683</v>
       </c>
       <c r="I109" s="245" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20187,7 +20189,7 @@
         <v>688</v>
       </c>
       <c r="I115" s="246" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20268,7 +20270,7 @@
         <v>35.32</v>
       </c>
       <c r="H119" s="247" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I119" s="88"/>
     </row>
@@ -20480,7 +20482,7 @@
         <v>55.55</v>
       </c>
       <c r="H129" s="248" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I129" s="88"/>
     </row>
@@ -20649,7 +20651,7 @@
         <v>716</v>
       </c>
       <c r="I137" s="249" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20687,7 +20689,7 @@
       </c>
       <c r="H139" s="88"/>
       <c r="I139" s="88" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20719,8 +20721,8 @@
         <f>+D140+1</f>
         <v>3</v>
       </c>
-      <c r="E141" s="117" t="s">
-        <v>719</v>
+      <c r="E141" s="258" t="s">
+        <v>1015</v>
       </c>
       <c r="F141" s="93">
         <f t="shared" ref="F141:F143" si="21">+G140</f>
@@ -20741,7 +20743,7 @@
         <v>4</v>
       </c>
       <c r="E142" s="117" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F142" s="93">
         <f t="shared" si="21"/>
@@ -20762,7 +20764,7 @@
         <v>5</v>
       </c>
       <c r="E143" s="117" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F143" s="93">
         <f t="shared" si="21"/>
@@ -20772,7 +20774,7 @@
         <v>55.42</v>
       </c>
       <c r="H143" s="250" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I143" s="88"/>
     </row>
@@ -20801,7 +20803,7 @@
         <v>1</v>
       </c>
       <c r="E145" s="119" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F145" s="93">
         <v>5.2</v>
@@ -20811,7 +20813,7 @@
       </c>
       <c r="H145" s="88"/>
       <c r="I145" s="88" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -20823,7 +20825,7 @@
         <v>2</v>
       </c>
       <c r="E146" s="119" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F146" s="93">
         <f>+G145</f>
@@ -20844,7 +20846,7 @@
         <v>3</v>
       </c>
       <c r="E147" s="119" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F147" s="93">
         <f t="shared" ref="F147:F162" si="23">+G146</f>
@@ -20865,7 +20867,7 @@
         <v>4</v>
       </c>
       <c r="E148" s="119" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F148" s="93">
         <f t="shared" si="23"/>
@@ -20886,7 +20888,7 @@
         <v>5</v>
       </c>
       <c r="E149" s="119" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F149" s="93">
         <f t="shared" si="23"/>
@@ -20907,7 +20909,7 @@
         <v>6</v>
       </c>
       <c r="E150" s="119" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F150" s="93">
         <f t="shared" si="23"/>
@@ -20928,7 +20930,7 @@
         <v>7</v>
       </c>
       <c r="E151" s="119" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F151" s="93">
         <f t="shared" si="23"/>
@@ -20949,7 +20951,7 @@
         <v>8</v>
       </c>
       <c r="E152" s="119" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F152" s="93">
         <f t="shared" si="23"/>
@@ -20970,7 +20972,7 @@
         <v>9</v>
       </c>
       <c r="E153" s="119" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F153" s="93">
         <f t="shared" si="23"/>
@@ -20991,7 +20993,7 @@
         <v>10</v>
       </c>
       <c r="E154" s="119" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F154" s="93">
         <f t="shared" si="23"/>
@@ -21012,7 +21014,7 @@
         <v>11</v>
       </c>
       <c r="E155" s="120" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F155" s="93">
         <f t="shared" si="23"/>
@@ -21033,7 +21035,7 @@
         <v>12</v>
       </c>
       <c r="E156" s="120" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F156" s="93">
         <f t="shared" si="23"/>
@@ -21054,7 +21056,7 @@
         <v>13</v>
       </c>
       <c r="E157" s="120" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F157" s="93">
         <f t="shared" si="23"/>
@@ -21075,7 +21077,7 @@
         <v>14</v>
       </c>
       <c r="E158" s="120" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F158" s="93">
         <f t="shared" si="23"/>
@@ -21096,7 +21098,7 @@
         <v>15</v>
       </c>
       <c r="E159" s="120" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F159" s="93">
         <f t="shared" si="23"/>
@@ -21117,7 +21119,7 @@
         <v>16</v>
       </c>
       <c r="E160" s="120" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F160" s="93">
         <f t="shared" si="23"/>
@@ -21138,7 +21140,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="120" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F161" s="93">
         <f t="shared" si="23"/>
@@ -21159,7 +21161,7 @@
         <v>18</v>
       </c>
       <c r="E162" s="120" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F162" s="93">
         <f t="shared" si="23"/>
@@ -21169,7 +21171,7 @@
         <v>58.49</v>
       </c>
       <c r="H162" s="251" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I162" s="88"/>
     </row>
@@ -22097,7 +22099,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="120" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F4" s="122">
         <v>2.1</v>
@@ -22107,7 +22109,7 @@
       </c>
       <c r="H4" s="120"/>
       <c r="I4" s="120" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22119,7 +22121,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="120" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F5" s="122">
         <f>+G4</f>
@@ -22140,7 +22142,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="123" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F6" s="122">
         <f>+G5</f>
@@ -22150,10 +22152,10 @@
         <v>52.3</v>
       </c>
       <c r="H6" s="124" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I6" s="253" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22181,7 +22183,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="124" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F8" s="122">
         <v>4.08</v>
@@ -22191,7 +22193,7 @@
       </c>
       <c r="H8" s="120"/>
       <c r="I8" s="120" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22203,7 +22205,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="124" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F9" s="122">
         <f>+G8</f>
@@ -22213,10 +22215,10 @@
         <v>49.5</v>
       </c>
       <c r="H9" s="124" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I9" s="254" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22243,7 +22245,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="124" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F11" s="120">
         <v>2.46</v>
@@ -22253,7 +22255,7 @@
       </c>
       <c r="H11" s="120"/>
       <c r="I11" s="120" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22265,7 +22267,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="124" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F12" s="120">
         <f>+G11</f>
@@ -22286,7 +22288,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="124" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F13" s="120">
         <f>+G12</f>
@@ -22307,7 +22309,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="125" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F14" s="120">
         <f>+G13</f>
@@ -22317,10 +22319,10 @@
         <v>57.3</v>
       </c>
       <c r="H14" s="125" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I14" s="254" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22348,7 +22350,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="125" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F16" s="120">
         <v>4.57</v>
@@ -22358,7 +22360,7 @@
       </c>
       <c r="H16" s="120"/>
       <c r="I16" s="120" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22370,7 +22372,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="125" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F17" s="120">
         <f>+G16</f>
@@ -22391,7 +22393,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="125" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F18" s="122">
         <f>+G17</f>
@@ -22402,7 +22404,7 @@
       </c>
       <c r="H18" s="120"/>
       <c r="I18" s="254" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22424,13 +22426,13 @@
         <v>44131</v>
       </c>
       <c r="C20" s="128" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D20" s="126">
         <v>1</v>
       </c>
       <c r="E20" s="127" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F20" s="122">
         <v>3.2</v>
@@ -22440,7 +22442,7 @@
       </c>
       <c r="H20" s="120"/>
       <c r="I20" s="120" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22452,7 +22454,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="127" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F21" s="122">
         <f>+G20</f>
@@ -22463,7 +22465,7 @@
       </c>
       <c r="H21" s="120"/>
       <c r="I21" s="254" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22475,7 +22477,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="127" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F22" s="122">
         <f>+G21</f>
@@ -22486,7 +22488,7 @@
       </c>
       <c r="H22" s="120"/>
       <c r="I22" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22514,7 +22516,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="129" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F24" s="120">
         <v>3.03</v>
@@ -22524,7 +22526,7 @@
       </c>
       <c r="H24" s="120"/>
       <c r="I24" s="120" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22536,7 +22538,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="129" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F25" s="120">
         <f>+G24</f>
@@ -22557,7 +22559,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="129" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F26" s="120">
         <f>+G25</f>
@@ -22567,10 +22569,10 @@
         <v>57.22</v>
       </c>
       <c r="H26" s="129" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I26" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22598,7 +22600,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="129" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F28" s="120">
         <v>4.29</v>
@@ -22608,7 +22610,7 @@
       </c>
       <c r="H28" s="120"/>
       <c r="I28" s="120" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22620,7 +22622,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="129" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F29" s="120">
         <f>+G28</f>
@@ -22641,7 +22643,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="129" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F30" s="120">
         <f t="shared" ref="F30:F31" si="0">+G29</f>
@@ -22662,7 +22664,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="130" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F31" s="120">
         <f t="shared" si="0"/>
@@ -22683,7 +22685,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="130" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F32" s="120">
         <f>+G31</f>
@@ -22693,10 +22695,10 @@
         <v>58.39</v>
       </c>
       <c r="H32" s="130" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I32" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22724,7 +22726,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="130" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F34" s="120">
         <v>4.16</v>
@@ -22734,7 +22736,7 @@
       </c>
       <c r="H34" s="120"/>
       <c r="I34" s="120" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22746,7 +22748,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="131" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F35" s="120">
         <f>+G34</f>
@@ -22767,7 +22769,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="131" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F36" s="120">
         <f t="shared" ref="F36" si="2">+G35</f>
@@ -22777,10 +22779,10 @@
         <v>44.45</v>
       </c>
       <c r="H36" s="132" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I36" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22808,7 +22810,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="132" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F38" s="120">
         <v>1.01</v>
@@ -22818,7 +22820,7 @@
       </c>
       <c r="H38" s="120"/>
       <c r="I38" s="120" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22830,7 +22832,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="132" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F39" s="120">
         <f>+G38</f>
@@ -22841,7 +22843,7 @@
       </c>
       <c r="H39" s="120"/>
       <c r="I39" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22853,7 +22855,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="132" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F40" s="122">
         <f>+G39</f>
@@ -22874,7 +22876,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="133" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F41" s="120">
         <f>+G40</f>
@@ -22884,10 +22886,10 @@
         <v>59.55</v>
       </c>
       <c r="H41" s="134" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="I41" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22909,13 +22911,13 @@
         <v>44136</v>
       </c>
       <c r="C43" s="134" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D43" s="126">
         <v>1</v>
       </c>
       <c r="E43" s="134" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F43" s="120">
         <v>3.12</v>
@@ -22925,7 +22927,7 @@
       </c>
       <c r="H43" s="120"/>
       <c r="I43" s="120" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22937,7 +22939,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="134" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F44" s="120">
         <f>+G43</f>
@@ -22958,7 +22960,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="134" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F45" s="120">
         <f t="shared" ref="F45" si="3">+G44</f>
@@ -22968,10 +22970,10 @@
         <v>59.05</v>
       </c>
       <c r="H45" s="134" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="I45" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -22996,7 +22998,7 @@
         <v>691</v>
       </c>
       <c r="E47" s="134" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F47" s="120">
         <v>4.5599999999999996</v>
@@ -23006,7 +23008,7 @@
       </c>
       <c r="H47" s="120"/>
       <c r="I47" s="120" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23014,7 +23016,7 @@
       <c r="B48" s="120"/>
       <c r="C48" s="120"/>
       <c r="E48" s="134" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F48" s="120">
         <f>+G47</f>
@@ -23031,7 +23033,7 @@
       <c r="B49" s="120"/>
       <c r="C49" s="120"/>
       <c r="E49" s="134" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F49" s="120">
         <f t="shared" ref="F49:F51" si="4">+G48</f>
@@ -23048,7 +23050,7 @@
       <c r="B50" s="120"/>
       <c r="C50" s="120"/>
       <c r="E50" s="134" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F50" s="120">
         <f t="shared" si="4"/>
@@ -23069,7 +23071,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="135" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F51" s="120">
         <f t="shared" si="4"/>
@@ -23079,10 +23081,10 @@
         <v>59.49</v>
       </c>
       <c r="H51" s="135" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="I51" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23104,13 +23106,13 @@
         <v>44138</v>
       </c>
       <c r="C53" s="136" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D53" s="126">
         <v>1</v>
       </c>
       <c r="E53" s="135" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F53" s="122">
         <v>6.3</v>
@@ -23120,7 +23122,7 @@
       </c>
       <c r="H53" s="120"/>
       <c r="I53" s="120" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23132,7 +23134,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="135" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F54" s="122">
         <f>+G53</f>
@@ -23153,7 +23155,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="135" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F55" s="122">
         <f t="shared" ref="F55:F56" si="5">+G54</f>
@@ -23174,18 +23176,18 @@
         <v>4</v>
       </c>
       <c r="E56" s="135" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F56" s="122">
         <f t="shared" si="5"/>
         <v>46.42</v>
       </c>
       <c r="G56" s="136" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H56" s="120"/>
       <c r="I56" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23213,7 +23215,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="136" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F58" s="120">
         <v>2.02</v>
@@ -23223,7 +23225,7 @@
       </c>
       <c r="H58" s="120"/>
       <c r="I58" s="120" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23235,7 +23237,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="136" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F59" s="120">
         <f>+G58</f>
@@ -23256,7 +23258,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="136" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F60" s="122">
         <f t="shared" ref="F60:F61" si="6">+G59</f>
@@ -23277,7 +23279,7 @@
         <v>4</v>
       </c>
       <c r="E61" s="137" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F61" s="122">
         <f t="shared" si="6"/>
@@ -23287,10 +23289,10 @@
         <v>58.4</v>
       </c>
       <c r="H61" s="138" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I61" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23318,7 +23320,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="138" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F63" s="120">
         <v>4.2300000000000004</v>
@@ -23328,7 +23330,7 @@
       </c>
       <c r="H63" s="120"/>
       <c r="I63" s="120" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23340,7 +23342,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="138" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F64" s="122">
         <f>+G63</f>
@@ -23361,7 +23363,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="138" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F65" s="122">
         <f>+G64</f>
@@ -23372,7 +23374,7 @@
       </c>
       <c r="H65" s="120"/>
       <c r="I65" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23400,7 +23402,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="138" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F67" s="122">
         <v>1.02</v>
@@ -23410,7 +23412,7 @@
       </c>
       <c r="H67" s="120"/>
       <c r="I67" s="120" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23422,7 +23424,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="138" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F68" s="120">
         <f>+G67</f>
@@ -23443,7 +23445,7 @@
         <v>3</v>
       </c>
       <c r="E69" s="138" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F69" s="120">
         <f t="shared" ref="F69:F70" si="7">+G68</f>
@@ -23464,7 +23466,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="138" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F70" s="120">
         <f t="shared" si="7"/>
@@ -23474,10 +23476,10 @@
         <v>51.33</v>
       </c>
       <c r="H70" s="139" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I70" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23505,7 +23507,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="139" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F72" s="139">
         <v>5.51</v>
@@ -23515,7 +23517,7 @@
       </c>
       <c r="H72" s="120"/>
       <c r="I72" s="120" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23527,7 +23529,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="139" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F73" s="120">
         <f>+G72</f>
@@ -23538,7 +23540,7 @@
       </c>
       <c r="H73" s="120"/>
       <c r="I73" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23550,7 +23552,7 @@
         <v>3</v>
       </c>
       <c r="E74" s="139" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F74" s="120">
         <f t="shared" ref="F74:F76" si="8">+G73</f>
@@ -23571,7 +23573,7 @@
         <v>4</v>
       </c>
       <c r="E75" s="139" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F75" s="120">
         <f t="shared" si="8"/>
@@ -23592,7 +23594,7 @@
         <v>5</v>
       </c>
       <c r="E76" s="139" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F76" s="120">
         <f t="shared" si="8"/>
@@ -23603,7 +23605,7 @@
       </c>
       <c r="H76" s="120"/>
       <c r="I76" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23631,7 +23633,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="139" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F78" s="120">
         <v>7.18</v>
@@ -23641,7 +23643,7 @@
       </c>
       <c r="H78" s="120"/>
       <c r="I78" s="120" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -23653,7 +23655,7 @@
         <v>2</v>
       </c>
       <c r="E79" s="139" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F79" s="120">
         <f>+G78</f>
@@ -23674,7 +23676,7 @@
         <v>3</v>
       </c>
       <c r="E80" s="139" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F80" s="120">
         <f t="shared" ref="F80:F81" si="9">+G79</f>
@@ -23695,7 +23697,7 @@
         <v>4</v>
       </c>
       <c r="E81" s="139" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F81" s="120">
         <f t="shared" si="9"/>
@@ -23706,7 +23708,7 @@
       </c>
       <c r="H81" s="120"/>
       <c r="I81" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -23734,7 +23736,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="140" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F83" s="120">
         <v>5.44</v>
@@ -23744,7 +23746,7 @@
       </c>
       <c r="H83" s="120"/>
       <c r="I83" s="120" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -23756,7 +23758,7 @@
         <v>2</v>
       </c>
       <c r="E84" s="140" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F84" s="120">
         <f>+G83</f>
@@ -23777,7 +23779,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="140" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F85" s="120">
         <f t="shared" ref="F85:F86" si="10">+G84</f>
@@ -23795,7 +23797,7 @@
         <v>4</v>
       </c>
       <c r="E86" s="140" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F86" s="120">
         <f t="shared" si="10"/>
@@ -23805,10 +23807,10 @@
         <v>58.18</v>
       </c>
       <c r="H86" s="140" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="I86" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.25">
@@ -23837,7 +23839,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="141" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F88" s="256">
         <v>0.57999999999999996</v>
@@ -23847,7 +23849,7 @@
       </c>
       <c r="H88" s="141"/>
       <c r="I88" s="141" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J88" s="141"/>
     </row>
@@ -23860,7 +23862,7 @@
         <v>2</v>
       </c>
       <c r="E89" s="141" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F89" s="141">
         <f>+G88</f>
@@ -23882,7 +23884,7 @@
         <v>3</v>
       </c>
       <c r="E90" s="141" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F90" s="141">
         <f>+G89</f>
@@ -23893,7 +23895,7 @@
       </c>
       <c r="H90" s="141"/>
       <c r="I90" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J90" s="141"/>
     </row>
@@ -23923,7 +23925,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="141" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F92" s="141">
         <v>2.11</v>
@@ -23933,7 +23935,7 @@
       </c>
       <c r="H92" s="141"/>
       <c r="I92" s="141" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="J92" s="141"/>
     </row>
@@ -23946,7 +23948,7 @@
         <v>2</v>
       </c>
       <c r="E93" s="141" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F93" s="141">
         <f>+G92</f>
@@ -23957,7 +23959,7 @@
       </c>
       <c r="H93" s="141"/>
       <c r="I93" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J93" s="141"/>
     </row>
@@ -23981,13 +23983,13 @@
         <v>44147</v>
       </c>
       <c r="C95" s="144" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D95" s="126">
         <v>1</v>
       </c>
       <c r="E95" s="143" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F95" s="141">
         <v>3.33</v>
@@ -23997,7 +23999,7 @@
       </c>
       <c r="H95" s="141"/>
       <c r="I95" s="141" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="J95" s="141"/>
     </row>
@@ -24010,7 +24012,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="143" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F96" s="141">
         <f>+G95</f>
@@ -24032,7 +24034,7 @@
         <v>3</v>
       </c>
       <c r="E97" s="143" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F97" s="145">
         <f t="shared" ref="F97:F101" si="11">+G96</f>
@@ -24054,7 +24056,7 @@
         <v>4</v>
       </c>
       <c r="E98" s="143" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F98" s="145">
         <f t="shared" si="11"/>
@@ -24076,7 +24078,7 @@
         <v>5</v>
       </c>
       <c r="E99" s="143" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F99" s="145">
         <f t="shared" si="11"/>
@@ -24087,7 +24089,7 @@
       </c>
       <c r="H99" s="141"/>
       <c r="I99" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J99" s="141"/>
     </row>
@@ -24100,7 +24102,7 @@
         <v>6</v>
       </c>
       <c r="E100" s="143" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F100" s="145">
         <f t="shared" si="11"/>
@@ -24122,18 +24124,18 @@
         <v>7</v>
       </c>
       <c r="E101" s="143" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="F101" s="145">
         <f t="shared" si="11"/>
         <v>48.56</v>
       </c>
       <c r="G101" s="143" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H101" s="141"/>
       <c r="I101" s="255" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J101" s="141"/>
     </row>
@@ -24284,7 +24286,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="143" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F3" s="143">
         <v>2.38</v>
@@ -24294,7 +24296,7 @@
       </c>
       <c r="H3" s="143"/>
       <c r="I3" s="143" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24306,7 +24308,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="143" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F4" s="143">
         <f>+G3</f>
@@ -24327,7 +24329,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="143" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F5" s="143">
         <f t="shared" ref="F5:F7" si="1">+G4</f>
@@ -24348,7 +24350,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="143" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F6" s="143">
         <f t="shared" si="1"/>
@@ -24369,7 +24371,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="148" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F7" s="143">
         <f t="shared" si="1"/>
@@ -24380,7 +24382,7 @@
       </c>
       <c r="H7" s="143"/>
       <c r="I7" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24408,7 +24410,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="149" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F9" s="143">
         <v>6.48</v>
@@ -24418,7 +24420,7 @@
       </c>
       <c r="H9" s="143"/>
       <c r="I9" s="143" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24430,7 +24432,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="149" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F10" s="143">
         <f>+G9</f>
@@ -24441,7 +24443,7 @@
       </c>
       <c r="H10" s="143"/>
       <c r="I10" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24469,7 +24471,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="149" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F12" s="143">
         <v>5.44</v>
@@ -24479,7 +24481,7 @@
       </c>
       <c r="H12" s="143"/>
       <c r="I12" s="143" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24491,7 +24493,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="149" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F13" s="143">
         <f>+G12</f>
@@ -24512,7 +24514,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="149" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F14" s="143">
         <f t="shared" ref="F14:F16" si="3">+G13</f>
@@ -24533,7 +24535,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="149" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F15" s="143">
         <f t="shared" si="3"/>
@@ -24554,7 +24556,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="149" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F16" s="143">
         <f t="shared" si="3"/>
@@ -24565,7 +24567,7 @@
       </c>
       <c r="H16" s="143"/>
       <c r="I16" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24593,7 +24595,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="151" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="F18" s="150">
         <v>5.2</v>
@@ -24603,7 +24605,7 @@
       </c>
       <c r="H18" s="143"/>
       <c r="I18" s="143" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24615,7 +24617,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="151" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F19" s="150">
         <f>+G18</f>
@@ -24636,7 +24638,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="151" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F20" s="150">
         <f t="shared" ref="F20:F26" si="5">+G19</f>
@@ -24657,7 +24659,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="151" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="F21" s="150">
         <f t="shared" si="5"/>
@@ -24678,7 +24680,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="151" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F22" s="150">
         <f t="shared" si="5"/>
@@ -24699,7 +24701,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="151" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F23" s="150">
         <f t="shared" si="5"/>
@@ -24720,7 +24722,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="151" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F24" s="150">
         <f t="shared" si="5"/>
@@ -24741,7 +24743,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="151" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F25" s="150">
         <f t="shared" si="5"/>
@@ -24762,7 +24764,7 @@
         <v>9</v>
       </c>
       <c r="E26" s="151" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F26" s="150">
         <f t="shared" si="5"/>
@@ -24773,7 +24775,7 @@
       </c>
       <c r="H26" s="143"/>
       <c r="I26" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24801,7 +24803,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="152" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F28" s="143">
         <v>7.27</v>
@@ -24811,7 +24813,7 @@
       </c>
       <c r="H28" s="143"/>
       <c r="I28" s="143" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24823,7 +24825,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="152" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F29" s="143">
         <f>+G28</f>
@@ -24844,7 +24846,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="152" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F30" s="143">
         <f t="shared" ref="F30:F31" si="7">+G29</f>
@@ -24865,7 +24867,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="152" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="F31" s="150">
         <f t="shared" si="7"/>
@@ -24876,7 +24878,7 @@
       </c>
       <c r="H31" s="143"/>
       <c r="I31" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24914,7 +24916,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="152" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="F34" s="143">
         <v>5.19</v>
@@ -24924,7 +24926,7 @@
       </c>
       <c r="H34" s="143"/>
       <c r="I34" s="143" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24936,7 +24938,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="152" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F35" s="150">
         <f>+G34</f>
@@ -24957,7 +24959,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="152" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="F36" s="150">
         <f>+G35</f>
@@ -24967,10 +24969,10 @@
         <v>41.52</v>
       </c>
       <c r="H36" s="154" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I36" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -24999,7 +25001,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="154" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F38" s="143">
         <v>2.4500000000000002</v>
@@ -25009,7 +25011,7 @@
       </c>
       <c r="H38" s="143"/>
       <c r="I38" s="143" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25021,7 +25023,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="154" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F39" s="143">
         <f>+G38</f>
@@ -25042,7 +25044,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="154" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="F40" s="143">
         <f>+G39</f>
@@ -25052,10 +25054,10 @@
         <v>39.090000000000003</v>
       </c>
       <c r="H40" s="154" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I40" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25084,7 +25086,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="154" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F42" s="143">
         <v>2.37</v>
@@ -25094,7 +25096,7 @@
       </c>
       <c r="H42" s="143"/>
       <c r="I42" s="143" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25106,7 +25108,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="154" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F43" s="150">
         <f>+G42</f>
@@ -25127,7 +25129,7 @@
         <v>3</v>
       </c>
       <c r="E44" s="154" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F44" s="150">
         <f t="shared" ref="F44:F54" si="11">+G43</f>
@@ -25148,7 +25150,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="154" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F45" s="150">
         <f t="shared" si="11"/>
@@ -25169,7 +25171,7 @@
         <v>5</v>
       </c>
       <c r="E46" s="154" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F46" s="150">
         <f t="shared" si="11"/>
@@ -25190,7 +25192,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="154" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F47" s="150">
         <f t="shared" si="11"/>
@@ -25211,7 +25213,7 @@
         <v>7</v>
       </c>
       <c r="E48" s="154" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F48" s="150">
         <f t="shared" si="11"/>
@@ -25232,7 +25234,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="155" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="F49" s="150">
         <f t="shared" si="11"/>
@@ -25253,7 +25255,7 @@
         <v>9</v>
       </c>
       <c r="E50" s="155" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F50" s="150">
         <f t="shared" si="11"/>
@@ -25274,7 +25276,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="155" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="F51" s="150">
         <f t="shared" si="11"/>
@@ -25295,7 +25297,7 @@
         <v>11</v>
       </c>
       <c r="E52" s="155" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="F52" s="150">
         <f t="shared" si="11"/>
@@ -25316,7 +25318,7 @@
         <v>12</v>
       </c>
       <c r="E53" s="155" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F53" s="150">
         <f t="shared" si="11"/>
@@ -25336,7 +25338,7 @@
         <v>13</v>
       </c>
       <c r="E54" s="155" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="F54" s="150">
         <f t="shared" si="11"/>
@@ -25346,10 +25348,10 @@
         <v>48.36</v>
       </c>
       <c r="H54" s="155" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I54" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25378,7 +25380,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="155" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F56" s="143">
         <v>2.04</v>
@@ -25388,7 +25390,7 @@
       </c>
       <c r="H56" s="143"/>
       <c r="I56" s="143" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25400,7 +25402,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="155" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F57" s="143">
         <f>+G56</f>
@@ -25421,7 +25423,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="155" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F58" s="143">
         <f t="shared" ref="F58:F61" si="13">+G57</f>
@@ -25442,7 +25444,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="155" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F59" s="143">
         <f t="shared" si="13"/>
@@ -25463,7 +25465,7 @@
         <v>5</v>
       </c>
       <c r="E60" s="155" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F60" s="143">
         <f t="shared" si="13"/>
@@ -25484,7 +25486,7 @@
         <v>6</v>
       </c>
       <c r="E61" s="156" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F61" s="143">
         <f t="shared" si="13"/>
@@ -25495,7 +25497,7 @@
       </c>
       <c r="H61" s="143"/>
       <c r="I61" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25534,7 +25536,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="156" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F64" s="143">
         <v>0.59</v>
@@ -25544,7 +25546,7 @@
       </c>
       <c r="H64" s="143"/>
       <c r="I64" s="143" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25556,7 +25558,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="156" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F65" s="150">
         <f>+G64</f>
@@ -25577,7 +25579,7 @@
         <v>3</v>
       </c>
       <c r="E66" s="156" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F66" s="150">
         <f t="shared" ref="F66:F67" si="15">+G65</f>
@@ -25598,7 +25600,7 @@
         <v>4</v>
       </c>
       <c r="E67" s="156" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F67" s="150">
         <f t="shared" si="15"/>
@@ -25608,10 +25610,10 @@
         <v>37.15</v>
       </c>
       <c r="H67" s="157" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="I67" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25640,7 +25642,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="157" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F69" s="143">
         <v>4.01</v>
@@ -25650,7 +25652,7 @@
       </c>
       <c r="H69" s="143"/>
       <c r="I69" s="143" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25662,7 +25664,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="157" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F70" s="143">
         <f>+G69</f>
@@ -25683,7 +25685,7 @@
         <v>3</v>
       </c>
       <c r="E71" s="157" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F71" s="143">
         <f t="shared" ref="F71:F74" si="16">+G70</f>
@@ -25704,7 +25706,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="157" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F72" s="150">
         <f t="shared" si="16"/>
@@ -25725,7 +25727,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="158" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F73" s="150">
         <f t="shared" si="16"/>
@@ -25746,7 +25748,7 @@
         <v>6</v>
       </c>
       <c r="E74" s="158" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F74" s="150">
         <f t="shared" si="16"/>
@@ -25757,7 +25759,7 @@
       </c>
       <c r="H74" s="143"/>
       <c r="I74" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25786,7 +25788,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="158" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F76" s="143">
         <v>1.44</v>
@@ -25796,7 +25798,7 @@
       </c>
       <c r="H76" s="143"/>
       <c r="I76" s="143" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25808,7 +25810,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="158" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F77" s="150">
         <f>+G76</f>
@@ -25829,7 +25831,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="158" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F78" s="150">
         <f t="shared" ref="F78:F81" si="18">+G77</f>
@@ -25850,7 +25852,7 @@
         <v>4</v>
       </c>
       <c r="E79" s="158" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F79" s="150">
         <f t="shared" si="18"/>
@@ -25871,7 +25873,7 @@
         <v>5</v>
       </c>
       <c r="E80" s="158" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F80" s="150">
         <f t="shared" si="18"/>
@@ -25892,7 +25894,7 @@
         <v>6</v>
       </c>
       <c r="E81" s="158" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F81" s="150">
         <f t="shared" si="18"/>
@@ -25903,7 +25905,7 @@
       </c>
       <c r="H81" s="143"/>
       <c r="I81" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25932,7 +25934,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="159" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F83" s="143">
         <v>3.57</v>
@@ -25942,7 +25944,7 @@
       </c>
       <c r="H83" s="143"/>
       <c r="I83" s="143" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -25954,7 +25956,7 @@
         <v>2</v>
       </c>
       <c r="E84" s="159" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F84" s="143">
         <f>+G83</f>
@@ -25975,7 +25977,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="159" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F85" s="143">
         <f t="shared" ref="F85" si="20">+G84</f>
@@ -25986,7 +25988,7 @@
       </c>
       <c r="H85" s="143"/>
       <c r="I85" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26015,7 +26017,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="159" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F87" s="143">
         <v>4.03</v>
@@ -26025,7 +26027,7 @@
       </c>
       <c r="H87" s="143"/>
       <c r="I87" s="143" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26037,7 +26039,7 @@
         <v>2</v>
       </c>
       <c r="E88" s="159" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F88" s="143">
         <f>+G87</f>
@@ -26047,10 +26049,10 @@
         <v>33.19</v>
       </c>
       <c r="H88" s="160" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I88" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26069,7 +26071,7 @@
         <v>15</v>
       </c>
       <c r="B90" s="161" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C90" s="143">
         <v>43.28</v>
@@ -26079,7 +26081,7 @@
         <v>1</v>
       </c>
       <c r="E90" s="161" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F90" s="143">
         <v>4.2699999999999996</v>
@@ -26089,7 +26091,7 @@
       </c>
       <c r="H90" s="143"/>
       <c r="I90" s="143" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26101,7 +26103,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="161" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F91" s="143">
         <f>+G90</f>
@@ -26121,7 +26123,7 @@
         <v>3</v>
       </c>
       <c r="E92" s="161" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F92" s="143">
         <f t="shared" ref="F92:F93" si="23">+G91</f>
@@ -26142,7 +26144,7 @@
         <v>4</v>
       </c>
       <c r="E93" s="161" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F93" s="143">
         <f t="shared" si="23"/>
@@ -26152,10 +26154,10 @@
         <v>42.22</v>
       </c>
       <c r="H93" s="162" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I93" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26184,7 +26186,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="162" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F95" s="143">
         <v>1.08</v>
@@ -26194,7 +26196,7 @@
       </c>
       <c r="H95" s="143"/>
       <c r="I95" s="143" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26206,7 +26208,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="162" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F96" s="143">
         <f>+G95</f>
@@ -26227,7 +26229,7 @@
         <v>3</v>
       </c>
       <c r="E97" s="162" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F97" s="143">
         <f t="shared" ref="F97:F100" si="25">+G96</f>
@@ -26248,7 +26250,7 @@
         <v>4</v>
       </c>
       <c r="E98" s="162" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F98" s="143">
         <f t="shared" si="25"/>
@@ -26269,7 +26271,7 @@
         <v>5</v>
       </c>
       <c r="E99" s="162" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F99" s="143">
         <f t="shared" si="25"/>
@@ -26290,7 +26292,7 @@
         <v>6</v>
       </c>
       <c r="E100" s="162" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="F100" s="143">
         <f t="shared" si="25"/>
@@ -26301,7 +26303,7 @@
       </c>
       <c r="H100" s="143"/>
       <c r="I100" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26320,7 +26322,7 @@
         <v>17</v>
       </c>
       <c r="B102" s="162" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C102" s="143">
         <v>47.38</v>
@@ -26330,7 +26332,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="162" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="F102" s="143">
         <v>3.16</v>
@@ -26340,7 +26342,7 @@
       </c>
       <c r="H102" s="143"/>
       <c r="I102" s="143" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26352,7 +26354,7 @@
         <v>2</v>
       </c>
       <c r="E103" s="162" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F103" s="143">
         <f>+G102</f>
@@ -26373,7 +26375,7 @@
         <v>3</v>
       </c>
       <c r="E104" s="162" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F104" s="143">
         <f t="shared" ref="F104:F111" si="27">+G103</f>
@@ -26394,7 +26396,7 @@
         <v>4</v>
       </c>
       <c r="E105" s="162" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F105" s="143">
         <f t="shared" si="27"/>
@@ -26415,7 +26417,7 @@
         <v>5</v>
       </c>
       <c r="E106" s="162" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F106" s="143">
         <f t="shared" si="27"/>
@@ -26436,7 +26438,7 @@
         <v>6</v>
       </c>
       <c r="E107" s="162" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F107" s="143">
         <f t="shared" si="27"/>
@@ -26457,7 +26459,7 @@
         <v>7</v>
       </c>
       <c r="E108" s="162" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F108" s="143">
         <f t="shared" si="27"/>
@@ -26478,7 +26480,7 @@
         <v>8</v>
       </c>
       <c r="E109" s="162" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F109" s="143">
         <f t="shared" si="27"/>
@@ -26499,7 +26501,7 @@
         <v>9</v>
       </c>
       <c r="E110" s="162" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F110" s="143">
         <f t="shared" si="27"/>
@@ -26520,7 +26522,7 @@
         <v>10</v>
       </c>
       <c r="E111" s="162" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F111" s="143">
         <f t="shared" si="27"/>
@@ -26531,7 +26533,7 @@
       </c>
       <c r="H111" s="143"/>
       <c r="I111" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26560,7 +26562,7 @@
         <v>1</v>
       </c>
       <c r="E113" s="163" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F113" s="143">
         <v>5.18</v>
@@ -26570,7 +26572,7 @@
       </c>
       <c r="H113" s="143"/>
       <c r="I113" s="143" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26582,7 +26584,7 @@
         <v>2</v>
       </c>
       <c r="E114" s="163" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F114" s="143">
         <f>+G113</f>
@@ -26603,7 +26605,7 @@
         <v>3</v>
       </c>
       <c r="E115" s="163" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F115" s="143">
         <f t="shared" ref="F115" si="29">+G114</f>
@@ -26614,7 +26616,7 @@
       </c>
       <c r="H115" s="143"/>
       <c r="I115" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26643,7 +26645,7 @@
         <v>1</v>
       </c>
       <c r="E117" s="164" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F117" s="143">
         <v>1.1200000000000001</v>
@@ -26653,7 +26655,7 @@
       </c>
       <c r="H117" s="143"/>
       <c r="I117" s="143" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26665,7 +26667,7 @@
         <v>2</v>
       </c>
       <c r="E118" s="164" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F118" s="143">
         <f>+G117</f>
@@ -26686,7 +26688,7 @@
         <v>3</v>
       </c>
       <c r="E119" s="164" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F119" s="143">
         <f t="shared" ref="F119:F120" si="30">+G118</f>
@@ -26707,7 +26709,7 @@
         <v>4</v>
       </c>
       <c r="E120" s="164" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F120" s="143">
         <f t="shared" si="30"/>
@@ -26718,7 +26720,7 @@
       </c>
       <c r="H120" s="143"/>
       <c r="I120" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26747,7 +26749,7 @@
         <v>1</v>
       </c>
       <c r="E122" s="165" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F122" s="143">
         <v>8.51</v>
@@ -26757,7 +26759,7 @@
       </c>
       <c r="H122" s="143"/>
       <c r="I122" s="143" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26769,7 +26771,7 @@
         <v>2</v>
       </c>
       <c r="E123" s="165" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F123" s="150">
         <f>+G122</f>
@@ -26780,7 +26782,7 @@
       </c>
       <c r="H123" s="143"/>
       <c r="I123" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26809,7 +26811,7 @@
         <v>1</v>
       </c>
       <c r="E125" s="166" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F125" s="167">
         <v>10.48</v>
@@ -26819,7 +26821,7 @@
       </c>
       <c r="H125" s="166"/>
       <c r="I125" s="166" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26831,7 +26833,7 @@
         <v>2</v>
       </c>
       <c r="E126" s="166" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F126" s="167">
         <f>+G125</f>
@@ -26852,7 +26854,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="166" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F127" s="167">
         <f t="shared" ref="F127:F128" si="33">+G126</f>
@@ -26873,7 +26875,7 @@
         <v>4</v>
       </c>
       <c r="E128" s="166" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F128" s="167">
         <f t="shared" si="33"/>
@@ -26884,7 +26886,7 @@
       </c>
       <c r="H128" s="166"/>
       <c r="I128" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26913,7 +26915,7 @@
         <v>1</v>
       </c>
       <c r="E130" s="166" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F130" s="166">
         <v>11.36</v>
@@ -26923,7 +26925,7 @@
       </c>
       <c r="H130" s="166"/>
       <c r="I130" s="166" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -26935,7 +26937,7 @@
         <v>2</v>
       </c>
       <c r="E131" s="166" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F131" s="167">
         <f>+G130</f>
@@ -26956,7 +26958,7 @@
         <v>3</v>
       </c>
       <c r="E132" s="166" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F132" s="167">
         <f t="shared" ref="F132:F136" si="34">+G131</f>
@@ -26977,7 +26979,7 @@
         <v>4</v>
       </c>
       <c r="E133" s="166" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F133" s="167">
         <f t="shared" si="34"/>
@@ -26998,7 +27000,7 @@
         <v>5</v>
       </c>
       <c r="E134" s="166" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="F134" s="167">
         <f t="shared" si="34"/>
@@ -27019,7 +27021,7 @@
         <v>6</v>
       </c>
       <c r="E135" s="166" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F135" s="167">
         <f t="shared" si="34"/>
@@ -27040,7 +27042,7 @@
         <v>7</v>
       </c>
       <c r="E136" s="169" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F136" s="167">
         <f t="shared" si="34"/>
@@ -27051,7 +27053,7 @@
       </c>
       <c r="H136" s="166"/>
       <c r="I136" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -27080,7 +27082,7 @@
         <v>1</v>
       </c>
       <c r="E138" s="166" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F138" s="167">
         <v>3.22</v>
@@ -27090,7 +27092,7 @@
       </c>
       <c r="H138" s="166"/>
       <c r="I138" s="166" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.25">
@@ -27102,7 +27104,7 @@
         <v>2</v>
       </c>
       <c r="E139" s="166" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F139" s="167">
         <f>+G138</f>
@@ -27123,7 +27125,7 @@
         <v>3</v>
       </c>
       <c r="E140" s="166" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F140" s="167">
         <f t="shared" ref="F140:F143" si="35">+G139</f>
@@ -27144,7 +27146,7 @@
         <v>4</v>
       </c>
       <c r="E141" s="166" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F141" s="167">
         <f t="shared" si="35"/>
@@ -27165,7 +27167,7 @@
         <v>5</v>
       </c>
       <c r="E142" s="166" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F142" s="167">
         <f t="shared" si="35"/>
@@ -27186,7 +27188,7 @@
         <v>6</v>
       </c>
       <c r="E143" s="166" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F143" s="167">
         <f t="shared" si="35"/>
@@ -27197,7 +27199,7 @@
       </c>
       <c r="H143" s="166"/>
       <c r="I143" s="257" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 27 07 2025
</commit_message>
<xml_diff>
--- a/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
+++ b/TS Jatai Working/TTD JatA PaaraayaNam-Jatai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D88EFE-DB94-4306-8DA7-95DBB0320793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222F8787-F31D-4502-B6C3-E15D3368DF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kandam1" sheetId="1" r:id="rId1"/>
@@ -17767,7 +17767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+    <sheetView topLeftCell="A142" workbookViewId="0">
       <selection activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
@@ -22009,8 +22009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>